<commit_message>
Update code fix bug print QPP011
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp011a.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/qpp011a.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="99">
   <si>
     <t>市区町村コード</t>
     <rPh sb="0" eb="2">
@@ -1074,30 +1074,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">    &amp;=$DBD_002                  市町村長殿　　　</t>
-    <rPh sb="32" eb="33">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>マチ</t>
-    </rPh>
-    <rPh sb="34" eb="35">
-      <t>ムラ</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>チョウ</t>
-    </rPh>
-    <rPh sb="36" eb="37">
-      <t>トノ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>&amp;=$DBD_012</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>&amp;=$DBD_014</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=$DBD_002   　　　</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>市町村長殿　　</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1442,7 +1431,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="206">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1545,6 +1534,30 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1730,24 +1743,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3038,8 +3033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="M4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="BQ14" sqref="BQ14:BZ15"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="M16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AS29" sqref="AS29:BE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3088,431 +3083,433 @@
     <row r="1" spans="1:80" ht="12.75" customHeight="1"/>
     <row r="2" spans="1:80" ht="12" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="49"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="57"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="150" t="s">
+      <c r="J2" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="151"/>
-      <c r="L2" s="151"/>
-      <c r="M2" s="151"/>
-      <c r="N2" s="151"/>
-      <c r="O2" s="151"/>
-      <c r="P2" s="151"/>
-      <c r="Q2" s="151"/>
-      <c r="R2" s="151"/>
-      <c r="S2" s="151"/>
-      <c r="T2" s="152"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
+      <c r="M2" s="153"/>
+      <c r="N2" s="153"/>
+      <c r="O2" s="153"/>
+      <c r="P2" s="153"/>
+      <c r="Q2" s="153"/>
+      <c r="R2" s="153"/>
+      <c r="S2" s="153"/>
+      <c r="T2" s="154"/>
       <c r="U2" s="4"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="49"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="56"/>
+      <c r="AA2" s="56"/>
+      <c r="AB2" s="56"/>
+      <c r="AC2" s="56"/>
+      <c r="AD2" s="57"/>
       <c r="AE2" s="3"/>
-      <c r="AF2" s="150" t="s">
+      <c r="AF2" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="AG2" s="151"/>
-      <c r="AH2" s="151"/>
-      <c r="AI2" s="151"/>
-      <c r="AJ2" s="151"/>
-      <c r="AK2" s="151"/>
-      <c r="AL2" s="151"/>
-      <c r="AM2" s="151"/>
-      <c r="AN2" s="151"/>
-      <c r="AO2" s="151"/>
-      <c r="AP2" s="152"/>
+      <c r="AG2" s="153"/>
+      <c r="AH2" s="153"/>
+      <c r="AI2" s="153"/>
+      <c r="AJ2" s="153"/>
+      <c r="AK2" s="153"/>
+      <c r="AL2" s="153"/>
+      <c r="AM2" s="153"/>
+      <c r="AN2" s="153"/>
+      <c r="AO2" s="153"/>
+      <c r="AP2" s="154"/>
       <c r="AQ2" s="4"/>
-      <c r="AS2" s="47"/>
-      <c r="AT2" s="48"/>
-      <c r="AU2" s="48"/>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="48"/>
-      <c r="AY2" s="48"/>
-      <c r="AZ2" s="49"/>
+      <c r="AS2" s="55"/>
+      <c r="AT2" s="56"/>
+      <c r="AU2" s="56"/>
+      <c r="AV2" s="56"/>
+      <c r="AW2" s="56"/>
+      <c r="AX2" s="56"/>
+      <c r="AY2" s="56"/>
+      <c r="AZ2" s="57"/>
       <c r="BA2" s="3"/>
-      <c r="BB2" s="150" t="s">
+      <c r="BB2" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="BC2" s="151"/>
-      <c r="BD2" s="151"/>
-      <c r="BE2" s="151"/>
-      <c r="BF2" s="151"/>
-      <c r="BG2" s="151"/>
-      <c r="BH2" s="151"/>
-      <c r="BI2" s="151"/>
-      <c r="BJ2" s="151"/>
-      <c r="BK2" s="151"/>
-      <c r="BL2" s="152"/>
+      <c r="BC2" s="153"/>
+      <c r="BD2" s="153"/>
+      <c r="BE2" s="153"/>
+      <c r="BF2" s="153"/>
+      <c r="BG2" s="153"/>
+      <c r="BH2" s="153"/>
+      <c r="BI2" s="153"/>
+      <c r="BJ2" s="153"/>
+      <c r="BK2" s="153"/>
+      <c r="BL2" s="154"/>
       <c r="BM2" s="4"/>
-      <c r="BO2" s="114" t="s">
+      <c r="BO2" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="BP2" s="91"/>
-      <c r="BQ2" s="117" t="s">
+      <c r="BP2" s="99"/>
+      <c r="BQ2" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="BR2" s="117"/>
-      <c r="BS2" s="117"/>
-      <c r="BT2" s="117"/>
-      <c r="BU2" s="117"/>
-      <c r="BV2" s="117"/>
-      <c r="BW2" s="117"/>
-      <c r="BX2" s="117"/>
-      <c r="BY2" s="117"/>
-      <c r="BZ2" s="118"/>
+      <c r="BR2" s="119"/>
+      <c r="BS2" s="119"/>
+      <c r="BT2" s="119"/>
+      <c r="BU2" s="119"/>
+      <c r="BV2" s="119"/>
+      <c r="BW2" s="119"/>
+      <c r="BX2" s="119"/>
+      <c r="BY2" s="119"/>
+      <c r="BZ2" s="120"/>
     </row>
     <row r="3" spans="1:80" ht="12.75" customHeight="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="60"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="50" t="s">
+      <c r="J3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51"/>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="51"/>
-      <c r="S3" s="51"/>
-      <c r="T3" s="52"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="60"/>
       <c r="U3" s="5"/>
-      <c r="W3" s="50"/>
-      <c r="X3" s="51"/>
-      <c r="Y3" s="51"/>
-      <c r="Z3" s="51"/>
-      <c r="AA3" s="51"/>
-      <c r="AB3" s="51"/>
-      <c r="AC3" s="51"/>
-      <c r="AD3" s="52"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59"/>
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="60"/>
       <c r="AE3" s="3"/>
-      <c r="AF3" s="50" t="s">
+      <c r="AF3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="51"/>
-      <c r="AK3" s="51"/>
-      <c r="AL3" s="51"/>
-      <c r="AM3" s="51"/>
-      <c r="AN3" s="51"/>
-      <c r="AO3" s="51"/>
-      <c r="AP3" s="52"/>
+      <c r="AG3" s="59"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="59"/>
+      <c r="AJ3" s="59"/>
+      <c r="AK3" s="59"/>
+      <c r="AL3" s="59"/>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="59"/>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="60"/>
       <c r="AQ3" s="5"/>
-      <c r="AS3" s="50"/>
-      <c r="AT3" s="51"/>
-      <c r="AU3" s="51"/>
-      <c r="AV3" s="51"/>
-      <c r="AW3" s="51"/>
-      <c r="AX3" s="51"/>
-      <c r="AY3" s="51"/>
-      <c r="AZ3" s="52"/>
+      <c r="AS3" s="58"/>
+      <c r="AT3" s="59"/>
+      <c r="AU3" s="59"/>
+      <c r="AV3" s="59"/>
+      <c r="AW3" s="59"/>
+      <c r="AX3" s="59"/>
+      <c r="AY3" s="59"/>
+      <c r="AZ3" s="60"/>
       <c r="BA3" s="3"/>
-      <c r="BB3" s="50" t="s">
+      <c r="BB3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="BC3" s="51"/>
-      <c r="BD3" s="51"/>
-      <c r="BE3" s="51"/>
-      <c r="BF3" s="51"/>
-      <c r="BG3" s="51"/>
-      <c r="BH3" s="51"/>
-      <c r="BI3" s="51"/>
-      <c r="BJ3" s="51"/>
-      <c r="BK3" s="51"/>
-      <c r="BL3" s="52"/>
+      <c r="BC3" s="59"/>
+      <c r="BD3" s="59"/>
+      <c r="BE3" s="59"/>
+      <c r="BF3" s="59"/>
+      <c r="BG3" s="59"/>
+      <c r="BH3" s="59"/>
+      <c r="BI3" s="59"/>
+      <c r="BJ3" s="59"/>
+      <c r="BK3" s="59"/>
+      <c r="BL3" s="60"/>
       <c r="BM3" s="5"/>
-      <c r="BO3" s="115"/>
-      <c r="BP3" s="116"/>
-      <c r="BQ3" s="119"/>
-      <c r="BR3" s="119"/>
-      <c r="BS3" s="119"/>
-      <c r="BT3" s="119"/>
-      <c r="BU3" s="119"/>
-      <c r="BV3" s="119"/>
-      <c r="BW3" s="119"/>
-      <c r="BX3" s="119"/>
-      <c r="BY3" s="119"/>
-      <c r="BZ3" s="120"/>
+      <c r="BO3" s="117"/>
+      <c r="BP3" s="118"/>
+      <c r="BQ3" s="121"/>
+      <c r="BR3" s="121"/>
+      <c r="BS3" s="121"/>
+      <c r="BT3" s="121"/>
+      <c r="BU3" s="121"/>
+      <c r="BV3" s="121"/>
+      <c r="BW3" s="121"/>
+      <c r="BX3" s="121"/>
+      <c r="BY3" s="121"/>
+      <c r="BZ3" s="122"/>
     </row>
     <row r="4" spans="1:80" ht="18.75">
       <c r="A4" s="2"/>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="55"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="63"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="153" t="s">
+      <c r="J4" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="154"/>
-      <c r="L4" s="154"/>
-      <c r="M4" s="154"/>
-      <c r="N4" s="154"/>
-      <c r="O4" s="154"/>
-      <c r="P4" s="154"/>
-      <c r="Q4" s="154"/>
-      <c r="R4" s="154"/>
-      <c r="S4" s="154"/>
-      <c r="T4" s="155"/>
+      <c r="K4" s="156"/>
+      <c r="L4" s="156"/>
+      <c r="M4" s="156"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="156"/>
+      <c r="Q4" s="156"/>
+      <c r="R4" s="156"/>
+      <c r="S4" s="156"/>
+      <c r="T4" s="157"/>
       <c r="U4" s="6"/>
-      <c r="W4" s="53"/>
-      <c r="X4" s="54"/>
-      <c r="Y4" s="54"/>
-      <c r="Z4" s="54"/>
-      <c r="AA4" s="54"/>
-      <c r="AB4" s="54"/>
-      <c r="AC4" s="54"/>
-      <c r="AD4" s="55"/>
+      <c r="W4" s="61"/>
+      <c r="X4" s="62"/>
+      <c r="Y4" s="62"/>
+      <c r="Z4" s="62"/>
+      <c r="AA4" s="62"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="62"/>
+      <c r="AD4" s="63"/>
       <c r="AE4" s="3"/>
-      <c r="AF4" s="153" t="s">
+      <c r="AF4" s="155" t="s">
         <v>12</v>
       </c>
-      <c r="AG4" s="154"/>
-      <c r="AH4" s="154"/>
-      <c r="AI4" s="154"/>
-      <c r="AJ4" s="154"/>
-      <c r="AK4" s="154"/>
-      <c r="AL4" s="154"/>
-      <c r="AM4" s="154"/>
-      <c r="AN4" s="154"/>
-      <c r="AO4" s="154"/>
-      <c r="AP4" s="155"/>
+      <c r="AG4" s="156"/>
+      <c r="AH4" s="156"/>
+      <c r="AI4" s="156"/>
+      <c r="AJ4" s="156"/>
+      <c r="AK4" s="156"/>
+      <c r="AL4" s="156"/>
+      <c r="AM4" s="156"/>
+      <c r="AN4" s="156"/>
+      <c r="AO4" s="156"/>
+      <c r="AP4" s="157"/>
       <c r="AQ4" s="6"/>
-      <c r="AS4" s="53"/>
-      <c r="AT4" s="54"/>
-      <c r="AU4" s="54"/>
-      <c r="AV4" s="54"/>
-      <c r="AW4" s="54"/>
-      <c r="AX4" s="54"/>
-      <c r="AY4" s="54"/>
-      <c r="AZ4" s="55"/>
+      <c r="AS4" s="61"/>
+      <c r="AT4" s="62"/>
+      <c r="AU4" s="62"/>
+      <c r="AV4" s="62"/>
+      <c r="AW4" s="62"/>
+      <c r="AX4" s="62"/>
+      <c r="AY4" s="62"/>
+      <c r="AZ4" s="63"/>
       <c r="BA4" s="3"/>
-      <c r="BB4" s="153" t="s">
+      <c r="BB4" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="BC4" s="154"/>
-      <c r="BD4" s="154"/>
-      <c r="BE4" s="154"/>
-      <c r="BF4" s="154"/>
-      <c r="BG4" s="154"/>
-      <c r="BH4" s="154"/>
-      <c r="BI4" s="154"/>
-      <c r="BJ4" s="154"/>
-      <c r="BK4" s="154"/>
-      <c r="BL4" s="155"/>
+      <c r="BC4" s="156"/>
+      <c r="BD4" s="156"/>
+      <c r="BE4" s="156"/>
+      <c r="BF4" s="156"/>
+      <c r="BG4" s="156"/>
+      <c r="BH4" s="156"/>
+      <c r="BI4" s="156"/>
+      <c r="BJ4" s="156"/>
+      <c r="BK4" s="156"/>
+      <c r="BL4" s="157"/>
       <c r="BM4" s="6"/>
-      <c r="BO4" s="93"/>
-      <c r="BP4" s="94"/>
-      <c r="BQ4" s="121"/>
-      <c r="BR4" s="121"/>
-      <c r="BS4" s="121"/>
-      <c r="BT4" s="121"/>
-      <c r="BU4" s="121"/>
-      <c r="BV4" s="121"/>
-      <c r="BW4" s="121"/>
-      <c r="BX4" s="121"/>
-      <c r="BY4" s="121"/>
-      <c r="BZ4" s="122"/>
+      <c r="BO4" s="101"/>
+      <c r="BP4" s="102"/>
+      <c r="BQ4" s="123"/>
+      <c r="BR4" s="123"/>
+      <c r="BS4" s="123"/>
+      <c r="BT4" s="123"/>
+      <c r="BU4" s="123"/>
+      <c r="BV4" s="123"/>
+      <c r="BW4" s="123"/>
+      <c r="BX4" s="123"/>
+      <c r="BY4" s="123"/>
+      <c r="BZ4" s="124"/>
       <c r="CB4" s="28"/>
     </row>
-    <row r="5" spans="1:80">
-      <c r="B5" s="144" t="s">
+    <row r="5" spans="1:80" ht="13.5" customHeight="1">
+      <c r="B5" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="145"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="145"/>
-      <c r="F5" s="145"/>
-      <c r="G5" s="145"/>
-      <c r="H5" s="146"/>
+      <c r="C5" s="147"/>
+      <c r="D5" s="147"/>
+      <c r="E5" s="147"/>
+      <c r="F5" s="147"/>
+      <c r="G5" s="147"/>
+      <c r="H5" s="148"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="156" t="s">
+      <c r="J5" s="158" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="157"/>
-      <c r="L5" s="157"/>
-      <c r="M5" s="157"/>
-      <c r="N5" s="157"/>
-      <c r="O5" s="157"/>
-      <c r="P5" s="157"/>
-      <c r="Q5" s="157"/>
-      <c r="R5" s="157"/>
-      <c r="S5" s="157"/>
-      <c r="T5" s="158"/>
+      <c r="K5" s="159"/>
+      <c r="L5" s="159"/>
+      <c r="M5" s="159"/>
+      <c r="N5" s="159"/>
+      <c r="O5" s="159"/>
+      <c r="P5" s="159"/>
+      <c r="Q5" s="159"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
+      <c r="T5" s="160"/>
       <c r="U5" s="5"/>
-      <c r="W5" s="144" t="s">
+      <c r="W5" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="X5" s="145"/>
-      <c r="Y5" s="145"/>
-      <c r="Z5" s="145"/>
-      <c r="AA5" s="145"/>
-      <c r="AB5" s="145"/>
-      <c r="AC5" s="145"/>
-      <c r="AD5" s="146"/>
+      <c r="X5" s="147"/>
+      <c r="Y5" s="147"/>
+      <c r="Z5" s="147"/>
+      <c r="AA5" s="147"/>
+      <c r="AB5" s="147"/>
+      <c r="AC5" s="147"/>
+      <c r="AD5" s="148"/>
       <c r="AE5" s="3"/>
-      <c r="AF5" s="156" t="s">
+      <c r="AF5" s="158" t="s">
         <v>72</v>
       </c>
-      <c r="AG5" s="157"/>
-      <c r="AH5" s="157"/>
-      <c r="AI5" s="157"/>
-      <c r="AJ5" s="157"/>
-      <c r="AK5" s="157"/>
-      <c r="AL5" s="157"/>
-      <c r="AM5" s="157"/>
-      <c r="AN5" s="157"/>
-      <c r="AO5" s="157"/>
-      <c r="AP5" s="158"/>
+      <c r="AG5" s="159"/>
+      <c r="AH5" s="159"/>
+      <c r="AI5" s="159"/>
+      <c r="AJ5" s="159"/>
+      <c r="AK5" s="159"/>
+      <c r="AL5" s="159"/>
+      <c r="AM5" s="159"/>
+      <c r="AN5" s="159"/>
+      <c r="AO5" s="159"/>
+      <c r="AP5" s="160"/>
       <c r="AQ5" s="5"/>
-      <c r="AS5" s="144" t="s">
+      <c r="AS5" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="AT5" s="145"/>
-      <c r="AU5" s="145"/>
-      <c r="AV5" s="145"/>
-      <c r="AW5" s="145"/>
-      <c r="AX5" s="145"/>
-      <c r="AY5" s="145"/>
-      <c r="AZ5" s="146"/>
+      <c r="AT5" s="147"/>
+      <c r="AU5" s="147"/>
+      <c r="AV5" s="147"/>
+      <c r="AW5" s="147"/>
+      <c r="AX5" s="147"/>
+      <c r="AY5" s="147"/>
+      <c r="AZ5" s="148"/>
       <c r="BA5" s="3"/>
-      <c r="BB5" s="156" t="s">
+      <c r="BB5" s="158" t="s">
         <v>57</v>
       </c>
-      <c r="BC5" s="157"/>
-      <c r="BD5" s="157"/>
-      <c r="BE5" s="157"/>
-      <c r="BF5" s="157"/>
-      <c r="BG5" s="157"/>
-      <c r="BH5" s="157"/>
-      <c r="BI5" s="157"/>
-      <c r="BJ5" s="157"/>
-      <c r="BK5" s="157"/>
-      <c r="BL5" s="158"/>
+      <c r="BC5" s="159"/>
+      <c r="BD5" s="159"/>
+      <c r="BE5" s="159"/>
+      <c r="BF5" s="159"/>
+      <c r="BG5" s="159"/>
+      <c r="BH5" s="159"/>
+      <c r="BI5" s="159"/>
+      <c r="BJ5" s="159"/>
+      <c r="BK5" s="159"/>
+      <c r="BL5" s="160"/>
       <c r="BM5" s="5"/>
-      <c r="BO5" s="96" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP5" s="97"/>
-      <c r="BQ5" s="97"/>
-      <c r="BR5" s="97"/>
-      <c r="BS5" s="97"/>
-      <c r="BT5" s="97"/>
-      <c r="BU5" s="97"/>
-      <c r="BV5" s="98"/>
-      <c r="BW5" s="105" t="s">
+      <c r="BO5" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="BP5" s="35"/>
+      <c r="BQ5" s="35"/>
+      <c r="BR5" s="35"/>
+      <c r="BS5" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="BT5" s="38"/>
+      <c r="BU5" s="38"/>
+      <c r="BV5" s="39"/>
+      <c r="BW5" s="107" t="s">
         <v>27</v>
       </c>
-      <c r="BX5" s="106"/>
-      <c r="BY5" s="106"/>
-      <c r="BZ5" s="107"/>
+      <c r="BX5" s="108"/>
+      <c r="BY5" s="108"/>
+      <c r="BZ5" s="109"/>
     </row>
     <row r="6" spans="1:80" ht="21.75" customHeight="1">
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="188" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="187"/>
-      <c r="D6" s="187"/>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="188"/>
+      <c r="C6" s="189"/>
+      <c r="D6" s="189"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="190"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="66"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="73"/>
+      <c r="R6" s="73"/>
+      <c r="S6" s="73"/>
+      <c r="T6" s="74"/>
       <c r="U6" s="5"/>
-      <c r="W6" s="186" t="s">
+      <c r="W6" s="188" t="s">
         <v>86</v>
       </c>
-      <c r="X6" s="187"/>
-      <c r="Y6" s="187"/>
-      <c r="Z6" s="187"/>
-      <c r="AA6" s="187"/>
-      <c r="AB6" s="187"/>
-      <c r="AC6" s="187"/>
-      <c r="AD6" s="188"/>
+      <c r="X6" s="189"/>
+      <c r="Y6" s="189"/>
+      <c r="Z6" s="189"/>
+      <c r="AA6" s="189"/>
+      <c r="AB6" s="189"/>
+      <c r="AC6" s="189"/>
+      <c r="AD6" s="190"/>
       <c r="AE6" s="3"/>
-      <c r="AF6" s="104"/>
-      <c r="AG6" s="65"/>
-      <c r="AH6" s="65"/>
-      <c r="AI6" s="65"/>
-      <c r="AJ6" s="65"/>
-      <c r="AK6" s="65"/>
-      <c r="AL6" s="65"/>
-      <c r="AM6" s="65"/>
-      <c r="AN6" s="65"/>
-      <c r="AO6" s="65"/>
-      <c r="AP6" s="66"/>
+      <c r="AF6" s="106"/>
+      <c r="AG6" s="73"/>
+      <c r="AH6" s="73"/>
+      <c r="AI6" s="73"/>
+      <c r="AJ6" s="73"/>
+      <c r="AK6" s="73"/>
+      <c r="AL6" s="73"/>
+      <c r="AM6" s="73"/>
+      <c r="AN6" s="73"/>
+      <c r="AO6" s="73"/>
+      <c r="AP6" s="74"/>
       <c r="AQ6" s="5"/>
-      <c r="AS6" s="186" t="s">
+      <c r="AS6" s="188" t="s">
         <v>85</v>
       </c>
-      <c r="AT6" s="187"/>
-      <c r="AU6" s="187"/>
-      <c r="AV6" s="187"/>
-      <c r="AW6" s="187"/>
-      <c r="AX6" s="187"/>
-      <c r="AY6" s="187"/>
-      <c r="AZ6" s="188"/>
+      <c r="AT6" s="189"/>
+      <c r="AU6" s="189"/>
+      <c r="AV6" s="189"/>
+      <c r="AW6" s="189"/>
+      <c r="AX6" s="189"/>
+      <c r="AY6" s="189"/>
+      <c r="AZ6" s="190"/>
       <c r="BA6" s="3"/>
-      <c r="BB6" s="104"/>
-      <c r="BC6" s="65"/>
-      <c r="BD6" s="65"/>
-      <c r="BE6" s="65"/>
-      <c r="BF6" s="65"/>
-      <c r="BG6" s="65"/>
-      <c r="BH6" s="65"/>
-      <c r="BI6" s="65"/>
-      <c r="BJ6" s="65"/>
-      <c r="BK6" s="65"/>
-      <c r="BL6" s="66"/>
+      <c r="BB6" s="106"/>
+      <c r="BC6" s="73"/>
+      <c r="BD6" s="73"/>
+      <c r="BE6" s="73"/>
+      <c r="BF6" s="73"/>
+      <c r="BG6" s="73"/>
+      <c r="BH6" s="73"/>
+      <c r="BI6" s="73"/>
+      <c r="BJ6" s="73"/>
+      <c r="BK6" s="73"/>
+      <c r="BL6" s="74"/>
       <c r="BM6" s="5"/>
-      <c r="BO6" s="99"/>
-      <c r="BP6" s="100"/>
-      <c r="BQ6" s="100"/>
-      <c r="BR6" s="100"/>
-      <c r="BS6" s="100"/>
-      <c r="BT6" s="100"/>
-      <c r="BU6" s="100"/>
-      <c r="BV6" s="101"/>
-      <c r="BW6" s="108"/>
-      <c r="BX6" s="109"/>
-      <c r="BY6" s="109"/>
-      <c r="BZ6" s="110"/>
+      <c r="BO6" s="36"/>
+      <c r="BP6" s="37"/>
+      <c r="BQ6" s="37"/>
+      <c r="BR6" s="37"/>
+      <c r="BS6" s="40"/>
+      <c r="BT6" s="40"/>
+      <c r="BU6" s="40"/>
+      <c r="BV6" s="41"/>
+      <c r="BW6" s="110"/>
+      <c r="BX6" s="111"/>
+      <c r="BY6" s="111"/>
+      <c r="BZ6" s="112"/>
     </row>
     <row r="7" spans="1:80">
       <c r="B7" s="3"/>
@@ -3577,196 +3574,196 @@
       <c r="BK7" s="3"/>
       <c r="BL7" s="3"/>
       <c r="BM7" s="7"/>
-      <c r="BO7" s="102" t="s">
+      <c r="BO7" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="BP7" s="63"/>
-      <c r="BQ7" s="63"/>
-      <c r="BR7" s="63"/>
-      <c r="BS7" s="63"/>
-      <c r="BT7" s="63"/>
-      <c r="BU7" s="63"/>
-      <c r="BV7" s="64"/>
-      <c r="BW7" s="108"/>
-      <c r="BX7" s="109"/>
-      <c r="BY7" s="109"/>
-      <c r="BZ7" s="110"/>
+      <c r="BP7" s="71"/>
+      <c r="BQ7" s="71"/>
+      <c r="BR7" s="71"/>
+      <c r="BS7" s="71"/>
+      <c r="BT7" s="71"/>
+      <c r="BU7" s="71"/>
+      <c r="BV7" s="72"/>
+      <c r="BW7" s="110"/>
+      <c r="BX7" s="111"/>
+      <c r="BY7" s="111"/>
+      <c r="BZ7" s="112"/>
     </row>
     <row r="8" spans="1:80">
-      <c r="B8" s="144" t="s">
+      <c r="B8" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="145"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="145"/>
-      <c r="F8" s="145"/>
-      <c r="G8" s="145"/>
-      <c r="H8" s="145"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="145"/>
-      <c r="K8" s="146"/>
-      <c r="L8" s="144" t="s">
+      <c r="C8" s="147"/>
+      <c r="D8" s="147"/>
+      <c r="E8" s="147"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
+      <c r="H8" s="147"/>
+      <c r="I8" s="147"/>
+      <c r="J8" s="147"/>
+      <c r="K8" s="148"/>
+      <c r="L8" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="145"/>
-      <c r="N8" s="145"/>
-      <c r="O8" s="145"/>
-      <c r="P8" s="145"/>
-      <c r="Q8" s="145"/>
-      <c r="R8" s="145"/>
-      <c r="S8" s="145"/>
-      <c r="T8" s="146"/>
+      <c r="M8" s="147"/>
+      <c r="N8" s="147"/>
+      <c r="O8" s="147"/>
+      <c r="P8" s="147"/>
+      <c r="Q8" s="147"/>
+      <c r="R8" s="147"/>
+      <c r="S8" s="147"/>
+      <c r="T8" s="148"/>
       <c r="U8" s="5"/>
-      <c r="W8" s="144" t="s">
+      <c r="W8" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="X8" s="145"/>
-      <c r="Y8" s="145"/>
-      <c r="Z8" s="145"/>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="145"/>
-      <c r="AC8" s="145"/>
-      <c r="AD8" s="145"/>
-      <c r="AE8" s="145"/>
-      <c r="AF8" s="145"/>
-      <c r="AG8" s="146"/>
-      <c r="AH8" s="144" t="s">
+      <c r="X8" s="147"/>
+      <c r="Y8" s="147"/>
+      <c r="Z8" s="147"/>
+      <c r="AA8" s="147"/>
+      <c r="AB8" s="147"/>
+      <c r="AC8" s="147"/>
+      <c r="AD8" s="147"/>
+      <c r="AE8" s="147"/>
+      <c r="AF8" s="147"/>
+      <c r="AG8" s="148"/>
+      <c r="AH8" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="AI8" s="145"/>
-      <c r="AJ8" s="145"/>
-      <c r="AK8" s="145"/>
-      <c r="AL8" s="145"/>
-      <c r="AM8" s="145"/>
-      <c r="AN8" s="145"/>
-      <c r="AO8" s="145"/>
-      <c r="AP8" s="146"/>
+      <c r="AI8" s="147"/>
+      <c r="AJ8" s="147"/>
+      <c r="AK8" s="147"/>
+      <c r="AL8" s="147"/>
+      <c r="AM8" s="147"/>
+      <c r="AN8" s="147"/>
+      <c r="AO8" s="147"/>
+      <c r="AP8" s="148"/>
       <c r="AQ8" s="5"/>
-      <c r="AS8" s="144" t="s">
+      <c r="AS8" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="AT8" s="145"/>
-      <c r="AU8" s="145"/>
-      <c r="AV8" s="145"/>
-      <c r="AW8" s="145"/>
-      <c r="AX8" s="145"/>
-      <c r="AY8" s="145"/>
-      <c r="AZ8" s="145"/>
-      <c r="BA8" s="145"/>
-      <c r="BB8" s="145"/>
-      <c r="BC8" s="146"/>
-      <c r="BD8" s="144" t="s">
+      <c r="AT8" s="147"/>
+      <c r="AU8" s="147"/>
+      <c r="AV8" s="147"/>
+      <c r="AW8" s="147"/>
+      <c r="AX8" s="147"/>
+      <c r="AY8" s="147"/>
+      <c r="AZ8" s="147"/>
+      <c r="BA8" s="147"/>
+      <c r="BB8" s="147"/>
+      <c r="BC8" s="148"/>
+      <c r="BD8" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="BE8" s="145"/>
-      <c r="BF8" s="145"/>
-      <c r="BG8" s="145"/>
-      <c r="BH8" s="145"/>
-      <c r="BI8" s="145"/>
-      <c r="BJ8" s="145"/>
-      <c r="BK8" s="145"/>
-      <c r="BL8" s="146"/>
+      <c r="BE8" s="147"/>
+      <c r="BF8" s="147"/>
+      <c r="BG8" s="147"/>
+      <c r="BH8" s="147"/>
+      <c r="BI8" s="147"/>
+      <c r="BJ8" s="147"/>
+      <c r="BK8" s="147"/>
+      <c r="BL8" s="148"/>
       <c r="BM8" s="5"/>
-      <c r="BO8" s="103"/>
-      <c r="BP8" s="63"/>
-      <c r="BQ8" s="63"/>
-      <c r="BR8" s="63"/>
-      <c r="BS8" s="63"/>
-      <c r="BT8" s="63"/>
-      <c r="BU8" s="63"/>
-      <c r="BV8" s="64"/>
-      <c r="BW8" s="108"/>
-      <c r="BX8" s="109"/>
-      <c r="BY8" s="109"/>
-      <c r="BZ8" s="110"/>
+      <c r="BO8" s="105"/>
+      <c r="BP8" s="71"/>
+      <c r="BQ8" s="71"/>
+      <c r="BR8" s="71"/>
+      <c r="BS8" s="71"/>
+      <c r="BT8" s="71"/>
+      <c r="BU8" s="71"/>
+      <c r="BV8" s="72"/>
+      <c r="BW8" s="110"/>
+      <c r="BX8" s="111"/>
+      <c r="BY8" s="111"/>
+      <c r="BZ8" s="112"/>
     </row>
     <row r="9" spans="1:80" ht="29.25" customHeight="1">
-      <c r="B9" s="186" t="s">
+      <c r="B9" s="188" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="187"/>
-      <c r="D9" s="187"/>
-      <c r="E9" s="187"/>
-      <c r="F9" s="187"/>
-      <c r="G9" s="187"/>
-      <c r="H9" s="187"/>
-      <c r="I9" s="187"/>
-      <c r="J9" s="187"/>
-      <c r="K9" s="188"/>
-      <c r="L9" s="203" t="s">
+      <c r="C9" s="189"/>
+      <c r="D9" s="189"/>
+      <c r="E9" s="189"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="189"/>
+      <c r="H9" s="189"/>
+      <c r="I9" s="189"/>
+      <c r="J9" s="189"/>
+      <c r="K9" s="190"/>
+      <c r="L9" s="205" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="204"/>
-      <c r="N9" s="204"/>
-      <c r="O9" s="204"/>
-      <c r="P9" s="204"/>
-      <c r="Q9" s="204"/>
-      <c r="R9" s="204"/>
-      <c r="S9" s="204"/>
-      <c r="T9" s="205"/>
+      <c r="M9" s="206"/>
+      <c r="N9" s="206"/>
+      <c r="O9" s="206"/>
+      <c r="P9" s="206"/>
+      <c r="Q9" s="206"/>
+      <c r="R9" s="206"/>
+      <c r="S9" s="206"/>
+      <c r="T9" s="207"/>
       <c r="U9" s="8"/>
-      <c r="W9" s="186" t="s">
+      <c r="W9" s="188" t="s">
         <v>58</v>
       </c>
-      <c r="X9" s="187"/>
-      <c r="Y9" s="187"/>
-      <c r="Z9" s="187"/>
-      <c r="AA9" s="187"/>
-      <c r="AB9" s="187"/>
-      <c r="AC9" s="187"/>
-      <c r="AD9" s="187"/>
-      <c r="AE9" s="187"/>
-      <c r="AF9" s="187"/>
-      <c r="AG9" s="188"/>
-      <c r="AH9" s="203" t="s">
+      <c r="X9" s="189"/>
+      <c r="Y9" s="189"/>
+      <c r="Z9" s="189"/>
+      <c r="AA9" s="189"/>
+      <c r="AB9" s="189"/>
+      <c r="AC9" s="189"/>
+      <c r="AD9" s="189"/>
+      <c r="AE9" s="189"/>
+      <c r="AF9" s="189"/>
+      <c r="AG9" s="190"/>
+      <c r="AH9" s="205" t="s">
         <v>60</v>
       </c>
-      <c r="AI9" s="204"/>
-      <c r="AJ9" s="204"/>
-      <c r="AK9" s="204"/>
-      <c r="AL9" s="204"/>
-      <c r="AM9" s="204"/>
-      <c r="AN9" s="204"/>
-      <c r="AO9" s="204"/>
-      <c r="AP9" s="205"/>
+      <c r="AI9" s="206"/>
+      <c r="AJ9" s="206"/>
+      <c r="AK9" s="206"/>
+      <c r="AL9" s="206"/>
+      <c r="AM9" s="206"/>
+      <c r="AN9" s="206"/>
+      <c r="AO9" s="206"/>
+      <c r="AP9" s="207"/>
       <c r="AQ9" s="8"/>
-      <c r="AS9" s="186" t="s">
+      <c r="AS9" s="188" t="s">
         <v>58</v>
       </c>
-      <c r="AT9" s="187"/>
-      <c r="AU9" s="187"/>
-      <c r="AV9" s="187"/>
-      <c r="AW9" s="187"/>
-      <c r="AX9" s="187"/>
-      <c r="AY9" s="187"/>
-      <c r="AZ9" s="187"/>
-      <c r="BA9" s="187"/>
-      <c r="BB9" s="187"/>
-      <c r="BC9" s="188"/>
-      <c r="BD9" s="203" t="s">
+      <c r="AT9" s="189"/>
+      <c r="AU9" s="189"/>
+      <c r="AV9" s="189"/>
+      <c r="AW9" s="189"/>
+      <c r="AX9" s="189"/>
+      <c r="AY9" s="189"/>
+      <c r="AZ9" s="189"/>
+      <c r="BA9" s="189"/>
+      <c r="BB9" s="189"/>
+      <c r="BC9" s="190"/>
+      <c r="BD9" s="205" t="s">
         <v>60</v>
       </c>
-      <c r="BE9" s="204"/>
-      <c r="BF9" s="204"/>
-      <c r="BG9" s="204"/>
-      <c r="BH9" s="204"/>
-      <c r="BI9" s="204"/>
-      <c r="BJ9" s="204"/>
-      <c r="BK9" s="204"/>
-      <c r="BL9" s="205"/>
+      <c r="BE9" s="206"/>
+      <c r="BF9" s="206"/>
+      <c r="BG9" s="206"/>
+      <c r="BH9" s="206"/>
+      <c r="BI9" s="206"/>
+      <c r="BJ9" s="206"/>
+      <c r="BK9" s="206"/>
+      <c r="BL9" s="207"/>
       <c r="BM9" s="8"/>
-      <c r="BO9" s="104"/>
-      <c r="BP9" s="65"/>
-      <c r="BQ9" s="65"/>
-      <c r="BR9" s="65"/>
-      <c r="BS9" s="65"/>
-      <c r="BT9" s="65"/>
-      <c r="BU9" s="65"/>
-      <c r="BV9" s="66"/>
-      <c r="BW9" s="111"/>
-      <c r="BX9" s="112"/>
-      <c r="BY9" s="112"/>
-      <c r="BZ9" s="113"/>
+      <c r="BO9" s="106"/>
+      <c r="BP9" s="73"/>
+      <c r="BQ9" s="73"/>
+      <c r="BR9" s="73"/>
+      <c r="BS9" s="73"/>
+      <c r="BT9" s="73"/>
+      <c r="BU9" s="73"/>
+      <c r="BV9" s="74"/>
+      <c r="BW9" s="113"/>
+      <c r="BX9" s="114"/>
+      <c r="BY9" s="114"/>
+      <c r="BZ9" s="115"/>
     </row>
     <row r="10" spans="1:80">
       <c r="B10" s="9"/>
@@ -3779,17 +3776,17 @@
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="11"/>
-      <c r="L10" s="144" t="s">
+      <c r="L10" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="145"/>
-      <c r="N10" s="145"/>
-      <c r="O10" s="145"/>
-      <c r="P10" s="145"/>
-      <c r="Q10" s="145"/>
-      <c r="R10" s="145"/>
-      <c r="S10" s="145"/>
-      <c r="T10" s="146"/>
+      <c r="M10" s="147"/>
+      <c r="N10" s="147"/>
+      <c r="O10" s="147"/>
+      <c r="P10" s="147"/>
+      <c r="Q10" s="147"/>
+      <c r="R10" s="147"/>
+      <c r="S10" s="147"/>
+      <c r="T10" s="148"/>
       <c r="U10" s="5"/>
       <c r="W10" s="9"/>
       <c r="X10" s="10"/>
@@ -3802,17 +3799,17 @@
       <c r="AE10" s="10"/>
       <c r="AF10" s="10"/>
       <c r="AG10" s="11"/>
-      <c r="AH10" s="144" t="s">
+      <c r="AH10" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="AI10" s="145"/>
-      <c r="AJ10" s="145"/>
-      <c r="AK10" s="145"/>
-      <c r="AL10" s="145"/>
-      <c r="AM10" s="145"/>
-      <c r="AN10" s="145"/>
-      <c r="AO10" s="145"/>
-      <c r="AP10" s="146"/>
+      <c r="AI10" s="147"/>
+      <c r="AJ10" s="147"/>
+      <c r="AK10" s="147"/>
+      <c r="AL10" s="147"/>
+      <c r="AM10" s="147"/>
+      <c r="AN10" s="147"/>
+      <c r="AO10" s="147"/>
+      <c r="AP10" s="148"/>
       <c r="AQ10" s="5"/>
       <c r="AS10" s="9"/>
       <c r="AT10" s="10"/>
@@ -3825,286 +3822,286 @@
       <c r="BA10" s="10"/>
       <c r="BB10" s="10"/>
       <c r="BC10" s="11"/>
-      <c r="BD10" s="144" t="s">
+      <c r="BD10" s="146" t="s">
         <v>9</v>
       </c>
-      <c r="BE10" s="145"/>
-      <c r="BF10" s="145"/>
-      <c r="BG10" s="145"/>
-      <c r="BH10" s="145"/>
-      <c r="BI10" s="145"/>
-      <c r="BJ10" s="145"/>
-      <c r="BK10" s="145"/>
-      <c r="BL10" s="146"/>
+      <c r="BE10" s="147"/>
+      <c r="BF10" s="147"/>
+      <c r="BG10" s="147"/>
+      <c r="BH10" s="147"/>
+      <c r="BI10" s="147"/>
+      <c r="BJ10" s="147"/>
+      <c r="BK10" s="147"/>
+      <c r="BL10" s="148"/>
       <c r="BM10" s="5"/>
-      <c r="BO10" s="34"/>
-      <c r="BP10" s="35"/>
-      <c r="BQ10" s="36"/>
-      <c r="BR10" s="34"/>
-      <c r="BS10" s="35"/>
-      <c r="BT10" s="36"/>
-      <c r="BU10" s="34"/>
-      <c r="BV10" s="35"/>
-      <c r="BW10" s="35"/>
-      <c r="BX10" s="35"/>
-      <c r="BY10" s="35"/>
-      <c r="BZ10" s="36"/>
+      <c r="BO10" s="42"/>
+      <c r="BP10" s="43"/>
+      <c r="BQ10" s="44"/>
+      <c r="BR10" s="42"/>
+      <c r="BS10" s="43"/>
+      <c r="BT10" s="44"/>
+      <c r="BU10" s="42"/>
+      <c r="BV10" s="43"/>
+      <c r="BW10" s="43"/>
+      <c r="BX10" s="43"/>
+      <c r="BY10" s="43"/>
+      <c r="BZ10" s="44"/>
     </row>
     <row r="11" spans="1:80" ht="15.75" customHeight="1">
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="180" t="s">
+      <c r="C11" s="71"/>
+      <c r="D11" s="71"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="182" t="s">
         <v>61</v>
       </c>
-      <c r="M11" s="181"/>
-      <c r="N11" s="181"/>
-      <c r="O11" s="181"/>
-      <c r="P11" s="181"/>
-      <c r="Q11" s="181"/>
-      <c r="R11" s="181"/>
-      <c r="S11" s="181"/>
-      <c r="T11" s="182"/>
+      <c r="M11" s="183"/>
+      <c r="N11" s="183"/>
+      <c r="O11" s="183"/>
+      <c r="P11" s="183"/>
+      <c r="Q11" s="183"/>
+      <c r="R11" s="183"/>
+      <c r="S11" s="183"/>
+      <c r="T11" s="184"/>
       <c r="U11" s="5"/>
-      <c r="W11" s="103" t="s">
+      <c r="W11" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="X11" s="63"/>
-      <c r="Y11" s="63"/>
-      <c r="Z11" s="63"/>
-      <c r="AA11" s="63"/>
-      <c r="AB11" s="63"/>
-      <c r="AC11" s="63"/>
-      <c r="AD11" s="63"/>
-      <c r="AE11" s="63"/>
-      <c r="AF11" s="63"/>
-      <c r="AG11" s="64"/>
-      <c r="AH11" s="180" t="s">
+      <c r="X11" s="71"/>
+      <c r="Y11" s="71"/>
+      <c r="Z11" s="71"/>
+      <c r="AA11" s="71"/>
+      <c r="AB11" s="71"/>
+      <c r="AC11" s="71"/>
+      <c r="AD11" s="71"/>
+      <c r="AE11" s="71"/>
+      <c r="AF11" s="71"/>
+      <c r="AG11" s="72"/>
+      <c r="AH11" s="182" t="s">
         <v>62</v>
       </c>
-      <c r="AI11" s="181"/>
-      <c r="AJ11" s="181"/>
-      <c r="AK11" s="181"/>
-      <c r="AL11" s="181"/>
-      <c r="AM11" s="181"/>
-      <c r="AN11" s="181"/>
-      <c r="AO11" s="181"/>
-      <c r="AP11" s="182"/>
+      <c r="AI11" s="183"/>
+      <c r="AJ11" s="183"/>
+      <c r="AK11" s="183"/>
+      <c r="AL11" s="183"/>
+      <c r="AM11" s="183"/>
+      <c r="AN11" s="183"/>
+      <c r="AO11" s="183"/>
+      <c r="AP11" s="184"/>
       <c r="AQ11" s="5"/>
-      <c r="AS11" s="103" t="s">
+      <c r="AS11" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="AT11" s="63"/>
-      <c r="AU11" s="63"/>
-      <c r="AV11" s="63"/>
-      <c r="AW11" s="63"/>
-      <c r="AX11" s="63"/>
-      <c r="AY11" s="63"/>
-      <c r="AZ11" s="63"/>
-      <c r="BA11" s="63"/>
-      <c r="BB11" s="63"/>
-      <c r="BC11" s="64"/>
-      <c r="BD11" s="180" t="s">
+      <c r="AT11" s="71"/>
+      <c r="AU11" s="71"/>
+      <c r="AV11" s="71"/>
+      <c r="AW11" s="71"/>
+      <c r="AX11" s="71"/>
+      <c r="AY11" s="71"/>
+      <c r="AZ11" s="71"/>
+      <c r="BA11" s="71"/>
+      <c r="BB11" s="71"/>
+      <c r="BC11" s="72"/>
+      <c r="BD11" s="182" t="s">
         <v>62</v>
       </c>
-      <c r="BE11" s="181"/>
-      <c r="BF11" s="181"/>
-      <c r="BG11" s="181"/>
-      <c r="BH11" s="181"/>
-      <c r="BI11" s="181"/>
-      <c r="BJ11" s="181"/>
-      <c r="BK11" s="181"/>
-      <c r="BL11" s="182"/>
+      <c r="BE11" s="183"/>
+      <c r="BF11" s="183"/>
+      <c r="BG11" s="183"/>
+      <c r="BH11" s="183"/>
+      <c r="BI11" s="183"/>
+      <c r="BJ11" s="183"/>
+      <c r="BK11" s="183"/>
+      <c r="BL11" s="184"/>
       <c r="BM11" s="5"/>
-      <c r="BO11" s="103" t="s">
+      <c r="BO11" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="BP11" s="63"/>
-      <c r="BQ11" s="64"/>
-      <c r="BR11" s="133" t="s">
+      <c r="BP11" s="71"/>
+      <c r="BQ11" s="72"/>
+      <c r="BR11" s="135" t="s">
         <v>21</v>
       </c>
-      <c r="BS11" s="135"/>
-      <c r="BT11" s="134"/>
-      <c r="BU11" s="128" t="s">
-        <v>97</v>
-      </c>
-      <c r="BV11" s="129"/>
-      <c r="BW11" s="129"/>
-      <c r="BX11" s="129"/>
-      <c r="BY11" s="129"/>
-      <c r="BZ11" s="130"/>
+      <c r="BS11" s="137"/>
+      <c r="BT11" s="136"/>
+      <c r="BU11" s="130" t="s">
+        <v>96</v>
+      </c>
+      <c r="BV11" s="131"/>
+      <c r="BW11" s="131"/>
+      <c r="BX11" s="131"/>
+      <c r="BY11" s="131"/>
+      <c r="BZ11" s="132"/>
     </row>
     <row r="12" spans="1:80">
-      <c r="B12" s="104"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="65"/>
-      <c r="H12" s="65"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="66"/>
-      <c r="L12" s="183"/>
-      <c r="M12" s="184"/>
-      <c r="N12" s="184"/>
-      <c r="O12" s="184"/>
-      <c r="P12" s="184"/>
-      <c r="Q12" s="184"/>
-      <c r="R12" s="184"/>
-      <c r="S12" s="184"/>
-      <c r="T12" s="185"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="185"/>
+      <c r="M12" s="186"/>
+      <c r="N12" s="186"/>
+      <c r="O12" s="186"/>
+      <c r="P12" s="186"/>
+      <c r="Q12" s="186"/>
+      <c r="R12" s="186"/>
+      <c r="S12" s="186"/>
+      <c r="T12" s="187"/>
       <c r="U12" s="5"/>
-      <c r="W12" s="104"/>
-      <c r="X12" s="65"/>
-      <c r="Y12" s="65"/>
-      <c r="Z12" s="65"/>
-      <c r="AA12" s="65"/>
-      <c r="AB12" s="65"/>
-      <c r="AC12" s="65"/>
-      <c r="AD12" s="65"/>
-      <c r="AE12" s="65"/>
-      <c r="AF12" s="65"/>
-      <c r="AG12" s="66"/>
-      <c r="AH12" s="183"/>
-      <c r="AI12" s="184"/>
-      <c r="AJ12" s="184"/>
-      <c r="AK12" s="184"/>
-      <c r="AL12" s="184"/>
-      <c r="AM12" s="184"/>
-      <c r="AN12" s="184"/>
-      <c r="AO12" s="184"/>
-      <c r="AP12" s="185"/>
+      <c r="W12" s="106"/>
+      <c r="X12" s="73"/>
+      <c r="Y12" s="73"/>
+      <c r="Z12" s="73"/>
+      <c r="AA12" s="73"/>
+      <c r="AB12" s="73"/>
+      <c r="AC12" s="73"/>
+      <c r="AD12" s="73"/>
+      <c r="AE12" s="73"/>
+      <c r="AF12" s="73"/>
+      <c r="AG12" s="74"/>
+      <c r="AH12" s="185"/>
+      <c r="AI12" s="186"/>
+      <c r="AJ12" s="186"/>
+      <c r="AK12" s="186"/>
+      <c r="AL12" s="186"/>
+      <c r="AM12" s="186"/>
+      <c r="AN12" s="186"/>
+      <c r="AO12" s="186"/>
+      <c r="AP12" s="187"/>
       <c r="AQ12" s="5"/>
-      <c r="AS12" s="104"/>
-      <c r="AT12" s="65"/>
-      <c r="AU12" s="65"/>
-      <c r="AV12" s="65"/>
-      <c r="AW12" s="65"/>
-      <c r="AX12" s="65"/>
-      <c r="AY12" s="65"/>
-      <c r="AZ12" s="65"/>
-      <c r="BA12" s="65"/>
-      <c r="BB12" s="65"/>
-      <c r="BC12" s="66"/>
-      <c r="BD12" s="183"/>
-      <c r="BE12" s="184"/>
-      <c r="BF12" s="184"/>
-      <c r="BG12" s="184"/>
-      <c r="BH12" s="184"/>
-      <c r="BI12" s="184"/>
-      <c r="BJ12" s="184"/>
-      <c r="BK12" s="184"/>
-      <c r="BL12" s="185"/>
+      <c r="AS12" s="106"/>
+      <c r="AT12" s="73"/>
+      <c r="AU12" s="73"/>
+      <c r="AV12" s="73"/>
+      <c r="AW12" s="73"/>
+      <c r="AX12" s="73"/>
+      <c r="AY12" s="73"/>
+      <c r="AZ12" s="73"/>
+      <c r="BA12" s="73"/>
+      <c r="BB12" s="73"/>
+      <c r="BC12" s="74"/>
+      <c r="BD12" s="185"/>
+      <c r="BE12" s="186"/>
+      <c r="BF12" s="186"/>
+      <c r="BG12" s="186"/>
+      <c r="BH12" s="186"/>
+      <c r="BI12" s="186"/>
+      <c r="BJ12" s="186"/>
+      <c r="BK12" s="186"/>
+      <c r="BL12" s="187"/>
       <c r="BM12" s="5"/>
-      <c r="BO12" s="104"/>
-      <c r="BP12" s="65"/>
-      <c r="BQ12" s="66"/>
-      <c r="BR12" s="70"/>
-      <c r="BS12" s="71"/>
-      <c r="BT12" s="72"/>
-      <c r="BU12" s="40"/>
-      <c r="BV12" s="41"/>
-      <c r="BW12" s="41"/>
-      <c r="BX12" s="41"/>
-      <c r="BY12" s="41"/>
-      <c r="BZ12" s="42"/>
+      <c r="BO12" s="106"/>
+      <c r="BP12" s="73"/>
+      <c r="BQ12" s="74"/>
+      <c r="BR12" s="78"/>
+      <c r="BS12" s="79"/>
+      <c r="BT12" s="80"/>
+      <c r="BU12" s="48"/>
+      <c r="BV12" s="49"/>
+      <c r="BW12" s="49"/>
+      <c r="BX12" s="49"/>
+      <c r="BY12" s="49"/>
+      <c r="BZ12" s="50"/>
     </row>
     <row r="13" spans="1:80" ht="7.5" customHeight="1">
-      <c r="B13" s="172" t="s">
+      <c r="B13" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="173"/>
-      <c r="D13" s="166" t="s">
+      <c r="C13" s="175"/>
+      <c r="D13" s="168" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="37" t="s">
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="38"/>
-      <c r="T13" s="39"/>
+      <c r="L13" s="46"/>
+      <c r="M13" s="46"/>
+      <c r="N13" s="46"/>
+      <c r="O13" s="46"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="46"/>
+      <c r="S13" s="46"/>
+      <c r="T13" s="47"/>
       <c r="U13" s="8"/>
-      <c r="W13" s="172" t="s">
+      <c r="W13" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="X13" s="173"/>
-      <c r="Y13" s="166" t="s">
+      <c r="X13" s="175"/>
+      <c r="Y13" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="Z13" s="167"/>
-      <c r="AA13" s="167"/>
-      <c r="AB13" s="167"/>
-      <c r="AC13" s="167"/>
-      <c r="AD13" s="167"/>
-      <c r="AE13" s="167"/>
-      <c r="AF13" s="168"/>
-      <c r="AG13" s="37" t="s">
+      <c r="Z13" s="169"/>
+      <c r="AA13" s="169"/>
+      <c r="AB13" s="169"/>
+      <c r="AC13" s="169"/>
+      <c r="AD13" s="169"/>
+      <c r="AE13" s="169"/>
+      <c r="AF13" s="170"/>
+      <c r="AG13" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="AH13" s="38"/>
-      <c r="AI13" s="38"/>
-      <c r="AJ13" s="38"/>
-      <c r="AK13" s="38"/>
-      <c r="AL13" s="38"/>
-      <c r="AM13" s="38"/>
-      <c r="AN13" s="38"/>
-      <c r="AO13" s="38"/>
-      <c r="AP13" s="39"/>
+      <c r="AH13" s="46"/>
+      <c r="AI13" s="46"/>
+      <c r="AJ13" s="46"/>
+      <c r="AK13" s="46"/>
+      <c r="AL13" s="46"/>
+      <c r="AM13" s="46"/>
+      <c r="AN13" s="46"/>
+      <c r="AO13" s="46"/>
+      <c r="AP13" s="47"/>
       <c r="AQ13" s="8"/>
-      <c r="AS13" s="172" t="s">
+      <c r="AS13" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="AT13" s="173"/>
-      <c r="AU13" s="166" t="s">
+      <c r="AT13" s="175"/>
+      <c r="AU13" s="168" t="s">
         <v>39</v>
       </c>
-      <c r="AV13" s="167"/>
-      <c r="AW13" s="167"/>
-      <c r="AX13" s="167"/>
-      <c r="AY13" s="167"/>
-      <c r="AZ13" s="167"/>
-      <c r="BA13" s="167"/>
-      <c r="BB13" s="168"/>
-      <c r="BC13" s="37" t="s">
+      <c r="AV13" s="169"/>
+      <c r="AW13" s="169"/>
+      <c r="AX13" s="169"/>
+      <c r="AY13" s="169"/>
+      <c r="AZ13" s="169"/>
+      <c r="BA13" s="169"/>
+      <c r="BB13" s="170"/>
+      <c r="BC13" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="BD13" s="38"/>
-      <c r="BE13" s="38"/>
-      <c r="BF13" s="38"/>
-      <c r="BG13" s="38"/>
-      <c r="BH13" s="38"/>
-      <c r="BI13" s="38"/>
-      <c r="BJ13" s="38"/>
-      <c r="BK13" s="38"/>
-      <c r="BL13" s="39"/>
+      <c r="BD13" s="46"/>
+      <c r="BE13" s="46"/>
+      <c r="BF13" s="46"/>
+      <c r="BG13" s="46"/>
+      <c r="BH13" s="46"/>
+      <c r="BI13" s="46"/>
+      <c r="BJ13" s="46"/>
+      <c r="BK13" s="46"/>
+      <c r="BL13" s="47"/>
       <c r="BM13" s="8"/>
-      <c r="BO13" s="131" t="s">
+      <c r="BO13" s="133" t="s">
         <v>34</v>
       </c>
-      <c r="BP13" s="132"/>
+      <c r="BP13" s="134"/>
       <c r="BQ13" s="14"/>
       <c r="BR13" s="12"/>
       <c r="BS13" s="12"/>
@@ -4117,1151 +4114,1151 @@
       <c r="BZ13" s="13"/>
     </row>
     <row r="14" spans="1:80" ht="16.5" customHeight="1">
-      <c r="B14" s="174"/>
-      <c r="C14" s="175"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="41"/>
-      <c r="R14" s="41"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="42"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="177"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="62"/>
+      <c r="J14" s="63"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49"/>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="49"/>
+      <c r="T14" s="50"/>
       <c r="U14" s="5"/>
-      <c r="W14" s="174"/>
-      <c r="X14" s="175"/>
-      <c r="Y14" s="169"/>
-      <c r="Z14" s="170"/>
-      <c r="AA14" s="170"/>
-      <c r="AB14" s="170"/>
-      <c r="AC14" s="170"/>
-      <c r="AD14" s="170"/>
-      <c r="AE14" s="170"/>
-      <c r="AF14" s="171"/>
-      <c r="AG14" s="40"/>
-      <c r="AH14" s="41"/>
-      <c r="AI14" s="41"/>
-      <c r="AJ14" s="41"/>
-      <c r="AK14" s="41"/>
-      <c r="AL14" s="41"/>
-      <c r="AM14" s="41"/>
-      <c r="AN14" s="41"/>
-      <c r="AO14" s="41"/>
-      <c r="AP14" s="42"/>
+      <c r="W14" s="176"/>
+      <c r="X14" s="177"/>
+      <c r="Y14" s="171"/>
+      <c r="Z14" s="172"/>
+      <c r="AA14" s="172"/>
+      <c r="AB14" s="172"/>
+      <c r="AC14" s="172"/>
+      <c r="AD14" s="172"/>
+      <c r="AE14" s="172"/>
+      <c r="AF14" s="173"/>
+      <c r="AG14" s="48"/>
+      <c r="AH14" s="49"/>
+      <c r="AI14" s="49"/>
+      <c r="AJ14" s="49"/>
+      <c r="AK14" s="49"/>
+      <c r="AL14" s="49"/>
+      <c r="AM14" s="49"/>
+      <c r="AN14" s="49"/>
+      <c r="AO14" s="49"/>
+      <c r="AP14" s="50"/>
       <c r="AQ14" s="5"/>
-      <c r="AS14" s="174"/>
-      <c r="AT14" s="175"/>
-      <c r="AU14" s="169"/>
-      <c r="AV14" s="170"/>
-      <c r="AW14" s="170"/>
-      <c r="AX14" s="170"/>
-      <c r="AY14" s="170"/>
-      <c r="AZ14" s="170"/>
-      <c r="BA14" s="170"/>
-      <c r="BB14" s="171"/>
-      <c r="BC14" s="40"/>
-      <c r="BD14" s="41"/>
-      <c r="BE14" s="41"/>
-      <c r="BF14" s="41"/>
-      <c r="BG14" s="41"/>
-      <c r="BH14" s="41"/>
-      <c r="BI14" s="41"/>
-      <c r="BJ14" s="41"/>
-      <c r="BK14" s="41"/>
-      <c r="BL14" s="42"/>
+      <c r="AS14" s="176"/>
+      <c r="AT14" s="177"/>
+      <c r="AU14" s="171"/>
+      <c r="AV14" s="172"/>
+      <c r="AW14" s="172"/>
+      <c r="AX14" s="172"/>
+      <c r="AY14" s="172"/>
+      <c r="AZ14" s="172"/>
+      <c r="BA14" s="172"/>
+      <c r="BB14" s="173"/>
+      <c r="BC14" s="48"/>
+      <c r="BD14" s="49"/>
+      <c r="BE14" s="49"/>
+      <c r="BF14" s="49"/>
+      <c r="BG14" s="49"/>
+      <c r="BH14" s="49"/>
+      <c r="BI14" s="49"/>
+      <c r="BJ14" s="49"/>
+      <c r="BK14" s="49"/>
+      <c r="BL14" s="50"/>
       <c r="BM14" s="5"/>
-      <c r="BO14" s="133"/>
-      <c r="BP14" s="134"/>
-      <c r="BQ14" s="128" t="s">
+      <c r="BO14" s="135"/>
+      <c r="BP14" s="136"/>
+      <c r="BQ14" s="130" t="s">
         <v>78</v>
       </c>
-      <c r="BR14" s="129"/>
-      <c r="BS14" s="129"/>
-      <c r="BT14" s="129"/>
-      <c r="BU14" s="129"/>
-      <c r="BV14" s="129"/>
-      <c r="BW14" s="129"/>
-      <c r="BX14" s="129"/>
-      <c r="BY14" s="129"/>
-      <c r="BZ14" s="130"/>
+      <c r="BR14" s="131"/>
+      <c r="BS14" s="131"/>
+      <c r="BT14" s="131"/>
+      <c r="BU14" s="131"/>
+      <c r="BV14" s="131"/>
+      <c r="BW14" s="131"/>
+      <c r="BX14" s="131"/>
+      <c r="BY14" s="131"/>
+      <c r="BZ14" s="132"/>
     </row>
     <row r="15" spans="1:80" ht="26.25" customHeight="1">
-      <c r="B15" s="174"/>
-      <c r="C15" s="175"/>
-      <c r="D15" s="163" t="s">
+      <c r="B15" s="176"/>
+      <c r="C15" s="177"/>
+      <c r="D15" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="164"/>
-      <c r="F15" s="164"/>
-      <c r="G15" s="164"/>
-      <c r="H15" s="164"/>
-      <c r="I15" s="164"/>
-      <c r="J15" s="165"/>
-      <c r="K15" s="160" t="s">
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="167"/>
+      <c r="K15" s="162" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="161"/>
-      <c r="M15" s="161"/>
-      <c r="N15" s="161"/>
-      <c r="O15" s="161"/>
-      <c r="P15" s="161"/>
-      <c r="Q15" s="161"/>
-      <c r="R15" s="161"/>
-      <c r="S15" s="161"/>
-      <c r="T15" s="162"/>
+      <c r="L15" s="163"/>
+      <c r="M15" s="163"/>
+      <c r="N15" s="163"/>
+      <c r="O15" s="163"/>
+      <c r="P15" s="163"/>
+      <c r="Q15" s="163"/>
+      <c r="R15" s="163"/>
+      <c r="S15" s="163"/>
+      <c r="T15" s="164"/>
       <c r="U15" s="5"/>
-      <c r="W15" s="174"/>
-      <c r="X15" s="175"/>
-      <c r="Y15" s="131" t="s">
+      <c r="W15" s="176"/>
+      <c r="X15" s="177"/>
+      <c r="Y15" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="Z15" s="159"/>
-      <c r="AA15" s="159"/>
-      <c r="AB15" s="159"/>
-      <c r="AC15" s="159"/>
-      <c r="AD15" s="159"/>
-      <c r="AE15" s="159"/>
-      <c r="AF15" s="132"/>
-      <c r="AG15" s="160" t="s">
+      <c r="Z15" s="161"/>
+      <c r="AA15" s="161"/>
+      <c r="AB15" s="161"/>
+      <c r="AC15" s="161"/>
+      <c r="AD15" s="161"/>
+      <c r="AE15" s="161"/>
+      <c r="AF15" s="134"/>
+      <c r="AG15" s="162" t="s">
         <v>64</v>
       </c>
-      <c r="AH15" s="161"/>
-      <c r="AI15" s="161"/>
-      <c r="AJ15" s="161"/>
-      <c r="AK15" s="161"/>
-      <c r="AL15" s="161"/>
-      <c r="AM15" s="161"/>
-      <c r="AN15" s="161"/>
-      <c r="AO15" s="161"/>
-      <c r="AP15" s="162"/>
+      <c r="AH15" s="163"/>
+      <c r="AI15" s="163"/>
+      <c r="AJ15" s="163"/>
+      <c r="AK15" s="163"/>
+      <c r="AL15" s="163"/>
+      <c r="AM15" s="163"/>
+      <c r="AN15" s="163"/>
+      <c r="AO15" s="163"/>
+      <c r="AP15" s="164"/>
       <c r="AQ15" s="5"/>
-      <c r="AS15" s="174"/>
-      <c r="AT15" s="175"/>
-      <c r="AU15" s="131" t="s">
+      <c r="AS15" s="176"/>
+      <c r="AT15" s="177"/>
+      <c r="AU15" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="AV15" s="159"/>
-      <c r="AW15" s="159"/>
-      <c r="AX15" s="159"/>
-      <c r="AY15" s="159"/>
-      <c r="AZ15" s="159"/>
-      <c r="BA15" s="159"/>
-      <c r="BB15" s="132"/>
-      <c r="BC15" s="160" t="s">
+      <c r="AV15" s="161"/>
+      <c r="AW15" s="161"/>
+      <c r="AX15" s="161"/>
+      <c r="AY15" s="161"/>
+      <c r="AZ15" s="161"/>
+      <c r="BA15" s="161"/>
+      <c r="BB15" s="134"/>
+      <c r="BC15" s="162" t="s">
         <v>64</v>
       </c>
-      <c r="BD15" s="161"/>
-      <c r="BE15" s="161"/>
-      <c r="BF15" s="161"/>
-      <c r="BG15" s="161"/>
-      <c r="BH15" s="161"/>
-      <c r="BI15" s="161"/>
-      <c r="BJ15" s="161"/>
-      <c r="BK15" s="161"/>
-      <c r="BL15" s="162"/>
+      <c r="BD15" s="163"/>
+      <c r="BE15" s="163"/>
+      <c r="BF15" s="163"/>
+      <c r="BG15" s="163"/>
+      <c r="BH15" s="163"/>
+      <c r="BI15" s="163"/>
+      <c r="BJ15" s="163"/>
+      <c r="BK15" s="163"/>
+      <c r="BL15" s="164"/>
       <c r="BM15" s="5"/>
-      <c r="BO15" s="70" t="s">
+      <c r="BO15" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="BP15" s="72"/>
-      <c r="BQ15" s="40"/>
-      <c r="BR15" s="41"/>
-      <c r="BS15" s="41"/>
-      <c r="BT15" s="41"/>
-      <c r="BU15" s="41"/>
-      <c r="BV15" s="41"/>
-      <c r="BW15" s="41"/>
-      <c r="BX15" s="41"/>
-      <c r="BY15" s="41"/>
-      <c r="BZ15" s="42"/>
+      <c r="BP15" s="80"/>
+      <c r="BQ15" s="48"/>
+      <c r="BR15" s="49"/>
+      <c r="BS15" s="49"/>
+      <c r="BT15" s="49"/>
+      <c r="BU15" s="49"/>
+      <c r="BV15" s="49"/>
+      <c r="BW15" s="49"/>
+      <c r="BX15" s="49"/>
+      <c r="BY15" s="49"/>
+      <c r="BZ15" s="50"/>
     </row>
     <row r="16" spans="1:80" ht="26.25" customHeight="1">
-      <c r="B16" s="174"/>
-      <c r="C16" s="175"/>
-      <c r="D16" s="163" t="s">
+      <c r="B16" s="176"/>
+      <c r="C16" s="177"/>
+      <c r="D16" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="164"/>
-      <c r="F16" s="164"/>
-      <c r="G16" s="164"/>
-      <c r="H16" s="164"/>
-      <c r="I16" s="164"/>
-      <c r="J16" s="165"/>
-      <c r="K16" s="160" t="s">
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="162" t="s">
         <v>65</v>
       </c>
-      <c r="L16" s="161"/>
-      <c r="M16" s="161"/>
-      <c r="N16" s="161"/>
-      <c r="O16" s="161"/>
-      <c r="P16" s="161"/>
-      <c r="Q16" s="161"/>
-      <c r="R16" s="161"/>
-      <c r="S16" s="161"/>
-      <c r="T16" s="162"/>
+      <c r="L16" s="163"/>
+      <c r="M16" s="163"/>
+      <c r="N16" s="163"/>
+      <c r="O16" s="163"/>
+      <c r="P16" s="163"/>
+      <c r="Q16" s="163"/>
+      <c r="R16" s="163"/>
+      <c r="S16" s="163"/>
+      <c r="T16" s="164"/>
       <c r="U16" s="5"/>
-      <c r="W16" s="174"/>
-      <c r="X16" s="175"/>
-      <c r="Y16" s="163" t="s">
+      <c r="W16" s="176"/>
+      <c r="X16" s="177"/>
+      <c r="Y16" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="Z16" s="164"/>
-      <c r="AA16" s="164"/>
-      <c r="AB16" s="164"/>
-      <c r="AC16" s="164"/>
-      <c r="AD16" s="164"/>
-      <c r="AE16" s="164"/>
-      <c r="AF16" s="165"/>
-      <c r="AG16" s="160" t="s">
+      <c r="Z16" s="166"/>
+      <c r="AA16" s="166"/>
+      <c r="AB16" s="166"/>
+      <c r="AC16" s="166"/>
+      <c r="AD16" s="166"/>
+      <c r="AE16" s="166"/>
+      <c r="AF16" s="167"/>
+      <c r="AG16" s="162" t="s">
         <v>74</v>
       </c>
-      <c r="AH16" s="161"/>
-      <c r="AI16" s="161"/>
-      <c r="AJ16" s="161"/>
-      <c r="AK16" s="161"/>
-      <c r="AL16" s="161"/>
-      <c r="AM16" s="161"/>
-      <c r="AN16" s="161"/>
-      <c r="AO16" s="161"/>
-      <c r="AP16" s="162"/>
+      <c r="AH16" s="163"/>
+      <c r="AI16" s="163"/>
+      <c r="AJ16" s="163"/>
+      <c r="AK16" s="163"/>
+      <c r="AL16" s="163"/>
+      <c r="AM16" s="163"/>
+      <c r="AN16" s="163"/>
+      <c r="AO16" s="163"/>
+      <c r="AP16" s="164"/>
       <c r="AQ16" s="5"/>
-      <c r="AS16" s="174"/>
-      <c r="AT16" s="175"/>
-      <c r="AU16" s="163" t="s">
+      <c r="AS16" s="176"/>
+      <c r="AT16" s="177"/>
+      <c r="AU16" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="AV16" s="164"/>
-      <c r="AW16" s="164"/>
-      <c r="AX16" s="164"/>
-      <c r="AY16" s="164"/>
-      <c r="AZ16" s="164"/>
-      <c r="BA16" s="164"/>
-      <c r="BB16" s="165"/>
-      <c r="BC16" s="160" t="s">
+      <c r="AV16" s="166"/>
+      <c r="AW16" s="166"/>
+      <c r="AX16" s="166"/>
+      <c r="AY16" s="166"/>
+      <c r="AZ16" s="166"/>
+      <c r="BA16" s="166"/>
+      <c r="BB16" s="167"/>
+      <c r="BC16" s="162" t="s">
         <v>66</v>
       </c>
-      <c r="BD16" s="161"/>
-      <c r="BE16" s="161"/>
-      <c r="BF16" s="161"/>
-      <c r="BG16" s="161"/>
-      <c r="BH16" s="161"/>
-      <c r="BI16" s="161"/>
-      <c r="BJ16" s="161"/>
-      <c r="BK16" s="161"/>
-      <c r="BL16" s="162"/>
+      <c r="BD16" s="163"/>
+      <c r="BE16" s="163"/>
+      <c r="BF16" s="163"/>
+      <c r="BG16" s="163"/>
+      <c r="BH16" s="163"/>
+      <c r="BI16" s="163"/>
+      <c r="BJ16" s="163"/>
+      <c r="BK16" s="163"/>
+      <c r="BL16" s="164"/>
       <c r="BM16" s="5"/>
       <c r="BO16" s="15"/>
-      <c r="BP16" s="126" t="s">
+      <c r="BP16" s="128" t="s">
         <v>24</v>
       </c>
-      <c r="BQ16" s="37" t="s">
+      <c r="BQ16" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="BR16" s="38"/>
-      <c r="BS16" s="38"/>
-      <c r="BT16" s="38"/>
-      <c r="BU16" s="38"/>
-      <c r="BV16" s="38"/>
-      <c r="BW16" s="38"/>
-      <c r="BX16" s="38"/>
-      <c r="BY16" s="38"/>
-      <c r="BZ16" s="39"/>
+      <c r="BR16" s="46"/>
+      <c r="BS16" s="46"/>
+      <c r="BT16" s="46"/>
+      <c r="BU16" s="46"/>
+      <c r="BV16" s="46"/>
+      <c r="BW16" s="46"/>
+      <c r="BX16" s="46"/>
+      <c r="BY16" s="46"/>
+      <c r="BZ16" s="47"/>
     </row>
     <row r="17" spans="2:78" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B17" s="174"/>
-      <c r="C17" s="175"/>
-      <c r="D17" s="131" t="s">
+      <c r="B17" s="176"/>
+      <c r="C17" s="177"/>
+      <c r="D17" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="159"/>
-      <c r="F17" s="159"/>
-      <c r="G17" s="159"/>
-      <c r="H17" s="159"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="132"/>
-      <c r="K17" s="37" t="s">
+      <c r="E17" s="161"/>
+      <c r="F17" s="161"/>
+      <c r="G17" s="161"/>
+      <c r="H17" s="161"/>
+      <c r="I17" s="161"/>
+      <c r="J17" s="134"/>
+      <c r="K17" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="38"/>
-      <c r="T17" s="39"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="47"/>
       <c r="U17" s="5"/>
-      <c r="W17" s="174"/>
-      <c r="X17" s="175"/>
-      <c r="Y17" s="131" t="s">
+      <c r="W17" s="176"/>
+      <c r="X17" s="177"/>
+      <c r="Y17" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="Z17" s="159"/>
-      <c r="AA17" s="159"/>
-      <c r="AB17" s="159"/>
-      <c r="AC17" s="159"/>
-      <c r="AD17" s="159"/>
-      <c r="AE17" s="159"/>
-      <c r="AF17" s="132"/>
-      <c r="AG17" s="37" t="s">
+      <c r="Z17" s="161"/>
+      <c r="AA17" s="161"/>
+      <c r="AB17" s="161"/>
+      <c r="AC17" s="161"/>
+      <c r="AD17" s="161"/>
+      <c r="AE17" s="161"/>
+      <c r="AF17" s="134"/>
+      <c r="AG17" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="AH17" s="38"/>
-      <c r="AI17" s="38"/>
-      <c r="AJ17" s="38"/>
-      <c r="AK17" s="38"/>
-      <c r="AL17" s="38"/>
-      <c r="AM17" s="38"/>
-      <c r="AN17" s="38"/>
-      <c r="AO17" s="38"/>
-      <c r="AP17" s="39"/>
+      <c r="AH17" s="46"/>
+      <c r="AI17" s="46"/>
+      <c r="AJ17" s="46"/>
+      <c r="AK17" s="46"/>
+      <c r="AL17" s="46"/>
+      <c r="AM17" s="46"/>
+      <c r="AN17" s="46"/>
+      <c r="AO17" s="46"/>
+      <c r="AP17" s="47"/>
       <c r="AQ17" s="5"/>
-      <c r="AS17" s="174"/>
-      <c r="AT17" s="175"/>
-      <c r="AU17" s="131" t="s">
+      <c r="AS17" s="176"/>
+      <c r="AT17" s="177"/>
+      <c r="AU17" s="133" t="s">
         <v>33</v>
       </c>
-      <c r="AV17" s="159"/>
-      <c r="AW17" s="159"/>
-      <c r="AX17" s="159"/>
-      <c r="AY17" s="159"/>
-      <c r="AZ17" s="159"/>
-      <c r="BA17" s="159"/>
-      <c r="BB17" s="132"/>
-      <c r="BC17" s="37" t="s">
+      <c r="AV17" s="161"/>
+      <c r="AW17" s="161"/>
+      <c r="AX17" s="161"/>
+      <c r="AY17" s="161"/>
+      <c r="AZ17" s="161"/>
+      <c r="BA17" s="161"/>
+      <c r="BB17" s="134"/>
+      <c r="BC17" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="BD17" s="38"/>
-      <c r="BE17" s="38"/>
-      <c r="BF17" s="38"/>
-      <c r="BG17" s="38"/>
-      <c r="BH17" s="38"/>
-      <c r="BI17" s="38"/>
-      <c r="BJ17" s="38"/>
-      <c r="BK17" s="38"/>
-      <c r="BL17" s="39"/>
+      <c r="BD17" s="46"/>
+      <c r="BE17" s="46"/>
+      <c r="BF17" s="46"/>
+      <c r="BG17" s="46"/>
+      <c r="BH17" s="46"/>
+      <c r="BI17" s="46"/>
+      <c r="BJ17" s="46"/>
+      <c r="BK17" s="46"/>
+      <c r="BL17" s="47"/>
       <c r="BM17" s="5"/>
       <c r="BO17" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="BP17" s="127"/>
-      <c r="BQ17" s="40"/>
-      <c r="BR17" s="41"/>
-      <c r="BS17" s="41"/>
-      <c r="BT17" s="41"/>
-      <c r="BU17" s="41"/>
-      <c r="BV17" s="41"/>
-      <c r="BW17" s="41"/>
-      <c r="BX17" s="41"/>
-      <c r="BY17" s="41"/>
-      <c r="BZ17" s="42"/>
+      <c r="BP17" s="129"/>
+      <c r="BQ17" s="48"/>
+      <c r="BR17" s="49"/>
+      <c r="BS17" s="49"/>
+      <c r="BT17" s="49"/>
+      <c r="BU17" s="49"/>
+      <c r="BV17" s="49"/>
+      <c r="BW17" s="49"/>
+      <c r="BX17" s="49"/>
+      <c r="BY17" s="49"/>
+      <c r="BZ17" s="50"/>
     </row>
     <row r="18" spans="2:78" ht="26.25" customHeight="1" thickBot="1">
-      <c r="B18" s="176"/>
-      <c r="C18" s="177"/>
-      <c r="D18" s="84" t="s">
+      <c r="B18" s="178"/>
+      <c r="C18" s="179"/>
+      <c r="D18" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="85"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="86"/>
-      <c r="K18" s="67" t="s">
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="93"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="68"/>
-      <c r="M18" s="68"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="68"/>
-      <c r="P18" s="68"/>
-      <c r="Q18" s="68"/>
-      <c r="R18" s="68"/>
-      <c r="S18" s="68"/>
-      <c r="T18" s="69"/>
+      <c r="L18" s="76"/>
+      <c r="M18" s="76"/>
+      <c r="N18" s="76"/>
+      <c r="O18" s="76"/>
+      <c r="P18" s="76"/>
+      <c r="Q18" s="76"/>
+      <c r="R18" s="76"/>
+      <c r="S18" s="76"/>
+      <c r="T18" s="77"/>
       <c r="U18" s="5"/>
-      <c r="W18" s="176"/>
-      <c r="X18" s="177"/>
-      <c r="Y18" s="84" t="s">
+      <c r="W18" s="178"/>
+      <c r="X18" s="179"/>
+      <c r="Y18" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="Z18" s="85"/>
-      <c r="AA18" s="85"/>
-      <c r="AB18" s="85"/>
-      <c r="AC18" s="85"/>
-      <c r="AD18" s="85"/>
-      <c r="AE18" s="85"/>
-      <c r="AF18" s="86"/>
-      <c r="AG18" s="67" t="s">
+      <c r="Z18" s="93"/>
+      <c r="AA18" s="93"/>
+      <c r="AB18" s="93"/>
+      <c r="AC18" s="93"/>
+      <c r="AD18" s="93"/>
+      <c r="AE18" s="93"/>
+      <c r="AF18" s="94"/>
+      <c r="AG18" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="AH18" s="68"/>
-      <c r="AI18" s="68"/>
-      <c r="AJ18" s="68"/>
-      <c r="AK18" s="68"/>
-      <c r="AL18" s="68"/>
-      <c r="AM18" s="68"/>
-      <c r="AN18" s="68"/>
-      <c r="AO18" s="68"/>
-      <c r="AP18" s="69"/>
+      <c r="AH18" s="76"/>
+      <c r="AI18" s="76"/>
+      <c r="AJ18" s="76"/>
+      <c r="AK18" s="76"/>
+      <c r="AL18" s="76"/>
+      <c r="AM18" s="76"/>
+      <c r="AN18" s="76"/>
+      <c r="AO18" s="76"/>
+      <c r="AP18" s="77"/>
       <c r="AQ18" s="5"/>
-      <c r="AS18" s="176"/>
-      <c r="AT18" s="177"/>
-      <c r="AU18" s="84" t="s">
+      <c r="AS18" s="178"/>
+      <c r="AT18" s="179"/>
+      <c r="AU18" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="AV18" s="85"/>
-      <c r="AW18" s="85"/>
-      <c r="AX18" s="85"/>
-      <c r="AY18" s="85"/>
-      <c r="AZ18" s="85"/>
-      <c r="BA18" s="85"/>
-      <c r="BB18" s="86"/>
-      <c r="BC18" s="67" t="s">
+      <c r="AV18" s="93"/>
+      <c r="AW18" s="93"/>
+      <c r="AX18" s="93"/>
+      <c r="AY18" s="93"/>
+      <c r="AZ18" s="93"/>
+      <c r="BA18" s="93"/>
+      <c r="BB18" s="94"/>
+      <c r="BC18" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="BD18" s="68"/>
-      <c r="BE18" s="68"/>
-      <c r="BF18" s="68"/>
-      <c r="BG18" s="68"/>
-      <c r="BH18" s="68"/>
-      <c r="BI18" s="68"/>
-      <c r="BJ18" s="68"/>
-      <c r="BK18" s="68"/>
-      <c r="BL18" s="69"/>
+      <c r="BD18" s="76"/>
+      <c r="BE18" s="76"/>
+      <c r="BF18" s="76"/>
+      <c r="BG18" s="76"/>
+      <c r="BH18" s="76"/>
+      <c r="BI18" s="76"/>
+      <c r="BJ18" s="76"/>
+      <c r="BK18" s="76"/>
+      <c r="BL18" s="77"/>
       <c r="BM18" s="5"/>
       <c r="BO18" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="BP18" s="126" t="s">
+      <c r="BP18" s="128" t="s">
         <v>25</v>
       </c>
-      <c r="BQ18" s="37" t="s">
+      <c r="BQ18" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="BR18" s="38"/>
-      <c r="BS18" s="38"/>
-      <c r="BT18" s="38"/>
-      <c r="BU18" s="38"/>
-      <c r="BV18" s="38"/>
-      <c r="BW18" s="38"/>
-      <c r="BX18" s="38"/>
-      <c r="BY18" s="38"/>
-      <c r="BZ18" s="39"/>
+      <c r="BR18" s="46"/>
+      <c r="BS18" s="46"/>
+      <c r="BT18" s="46"/>
+      <c r="BU18" s="46"/>
+      <c r="BV18" s="46"/>
+      <c r="BW18" s="46"/>
+      <c r="BX18" s="46"/>
+      <c r="BY18" s="46"/>
+      <c r="BZ18" s="47"/>
     </row>
     <row r="19" spans="2:78" ht="20.25" customHeight="1">
-      <c r="B19" s="70" t="s">
+      <c r="B19" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="191" t="s">
+      <c r="C19" s="79"/>
+      <c r="D19" s="79"/>
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="193" t="s">
         <v>54</v>
       </c>
-      <c r="J19" s="192"/>
-      <c r="K19" s="192"/>
-      <c r="L19" s="192"/>
-      <c r="M19" s="192"/>
-      <c r="N19" s="192"/>
-      <c r="O19" s="192"/>
-      <c r="P19" s="192"/>
-      <c r="Q19" s="192"/>
-      <c r="R19" s="192"/>
-      <c r="S19" s="192"/>
-      <c r="T19" s="193"/>
+      <c r="J19" s="194"/>
+      <c r="K19" s="194"/>
+      <c r="L19" s="194"/>
+      <c r="M19" s="194"/>
+      <c r="N19" s="194"/>
+      <c r="O19" s="194"/>
+      <c r="P19" s="194"/>
+      <c r="Q19" s="194"/>
+      <c r="R19" s="194"/>
+      <c r="S19" s="194"/>
+      <c r="T19" s="195"/>
       <c r="U19" s="5"/>
-      <c r="W19" s="70" t="s">
+      <c r="W19" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="X19" s="71"/>
-      <c r="Y19" s="71"/>
-      <c r="Z19" s="71"/>
-      <c r="AA19" s="71"/>
-      <c r="AB19" s="71"/>
-      <c r="AC19" s="71"/>
-      <c r="AD19" s="72"/>
-      <c r="AE19" s="70" t="s">
+      <c r="X19" s="79"/>
+      <c r="Y19" s="79"/>
+      <c r="Z19" s="79"/>
+      <c r="AA19" s="79"/>
+      <c r="AB19" s="79"/>
+      <c r="AC19" s="79"/>
+      <c r="AD19" s="80"/>
+      <c r="AE19" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="AF19" s="71"/>
-      <c r="AG19" s="71"/>
-      <c r="AH19" s="71"/>
-      <c r="AI19" s="71"/>
-      <c r="AJ19" s="71"/>
-      <c r="AK19" s="71"/>
-      <c r="AL19" s="71"/>
-      <c r="AM19" s="71"/>
-      <c r="AN19" s="71"/>
-      <c r="AO19" s="71"/>
-      <c r="AP19" s="72"/>
+      <c r="AF19" s="79"/>
+      <c r="AG19" s="79"/>
+      <c r="AH19" s="79"/>
+      <c r="AI19" s="79"/>
+      <c r="AJ19" s="79"/>
+      <c r="AK19" s="79"/>
+      <c r="AL19" s="79"/>
+      <c r="AM19" s="79"/>
+      <c r="AN19" s="79"/>
+      <c r="AO19" s="79"/>
+      <c r="AP19" s="80"/>
       <c r="AQ19" s="5"/>
-      <c r="AS19" s="70" t="s">
+      <c r="AS19" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="AT19" s="71"/>
-      <c r="AU19" s="71"/>
-      <c r="AV19" s="71"/>
-      <c r="AW19" s="71"/>
-      <c r="AX19" s="71"/>
-      <c r="AY19" s="71"/>
-      <c r="AZ19" s="72"/>
-      <c r="BA19" s="70" t="s">
+      <c r="AT19" s="79"/>
+      <c r="AU19" s="79"/>
+      <c r="AV19" s="79"/>
+      <c r="AW19" s="79"/>
+      <c r="AX19" s="79"/>
+      <c r="AY19" s="79"/>
+      <c r="AZ19" s="80"/>
+      <c r="BA19" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="BB19" s="71"/>
-      <c r="BC19" s="71"/>
-      <c r="BD19" s="71"/>
-      <c r="BE19" s="71"/>
-      <c r="BF19" s="71"/>
-      <c r="BG19" s="71"/>
-      <c r="BH19" s="71"/>
-      <c r="BI19" s="71"/>
-      <c r="BJ19" s="71"/>
-      <c r="BK19" s="71"/>
-      <c r="BL19" s="72"/>
+      <c r="BB19" s="79"/>
+      <c r="BC19" s="79"/>
+      <c r="BD19" s="79"/>
+      <c r="BE19" s="79"/>
+      <c r="BF19" s="79"/>
+      <c r="BG19" s="79"/>
+      <c r="BH19" s="79"/>
+      <c r="BI19" s="79"/>
+      <c r="BJ19" s="79"/>
+      <c r="BK19" s="79"/>
+      <c r="BL19" s="80"/>
       <c r="BM19" s="5"/>
       <c r="BO19" s="17"/>
-      <c r="BP19" s="127"/>
-      <c r="BQ19" s="40"/>
-      <c r="BR19" s="41"/>
-      <c r="BS19" s="41"/>
-      <c r="BT19" s="41"/>
-      <c r="BU19" s="41"/>
-      <c r="BV19" s="41"/>
-      <c r="BW19" s="41"/>
-      <c r="BX19" s="41"/>
-      <c r="BY19" s="41"/>
-      <c r="BZ19" s="42"/>
+      <c r="BP19" s="129"/>
+      <c r="BQ19" s="48"/>
+      <c r="BR19" s="49"/>
+      <c r="BS19" s="49"/>
+      <c r="BT19" s="49"/>
+      <c r="BU19" s="49"/>
+      <c r="BV19" s="49"/>
+      <c r="BW19" s="49"/>
+      <c r="BX19" s="49"/>
+      <c r="BY19" s="49"/>
+      <c r="BZ19" s="50"/>
     </row>
     <row r="20" spans="2:78" ht="10.5" customHeight="1">
-      <c r="B20" s="87" t="s">
+      <c r="B20" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="88"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="88"/>
-      <c r="O20" s="88"/>
-      <c r="P20" s="88"/>
-      <c r="Q20" s="88"/>
-      <c r="R20" s="88"/>
-      <c r="S20" s="88"/>
-      <c r="T20" s="89"/>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="96"/>
+      <c r="J20" s="96"/>
+      <c r="K20" s="96"/>
+      <c r="L20" s="96"/>
+      <c r="M20" s="96"/>
+      <c r="N20" s="96"/>
+      <c r="O20" s="96"/>
+      <c r="P20" s="96"/>
+      <c r="Q20" s="96"/>
+      <c r="R20" s="96"/>
+      <c r="S20" s="96"/>
+      <c r="T20" s="97"/>
       <c r="U20" s="18"/>
-      <c r="W20" s="87" t="s">
+      <c r="W20" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="X20" s="88"/>
-      <c r="Y20" s="88"/>
-      <c r="Z20" s="88"/>
-      <c r="AA20" s="88"/>
-      <c r="AB20" s="88"/>
-      <c r="AC20" s="88"/>
-      <c r="AD20" s="88"/>
-      <c r="AE20" s="88"/>
-      <c r="AF20" s="88"/>
-      <c r="AG20" s="88"/>
-      <c r="AH20" s="88"/>
-      <c r="AI20" s="88"/>
-      <c r="AJ20" s="88"/>
-      <c r="AK20" s="88"/>
-      <c r="AL20" s="88"/>
-      <c r="AM20" s="88"/>
-      <c r="AN20" s="88"/>
-      <c r="AO20" s="88"/>
-      <c r="AP20" s="89"/>
+      <c r="X20" s="96"/>
+      <c r="Y20" s="96"/>
+      <c r="Z20" s="96"/>
+      <c r="AA20" s="96"/>
+      <c r="AB20" s="96"/>
+      <c r="AC20" s="96"/>
+      <c r="AD20" s="96"/>
+      <c r="AE20" s="96"/>
+      <c r="AF20" s="96"/>
+      <c r="AG20" s="96"/>
+      <c r="AH20" s="96"/>
+      <c r="AI20" s="96"/>
+      <c r="AJ20" s="96"/>
+      <c r="AK20" s="96"/>
+      <c r="AL20" s="96"/>
+      <c r="AM20" s="96"/>
+      <c r="AN20" s="96"/>
+      <c r="AO20" s="96"/>
+      <c r="AP20" s="97"/>
       <c r="AQ20" s="18"/>
-      <c r="AS20" s="87" t="s">
+      <c r="AS20" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="AT20" s="88"/>
-      <c r="AU20" s="88"/>
-      <c r="AV20" s="88"/>
-      <c r="AW20" s="88"/>
-      <c r="AX20" s="88"/>
-      <c r="AY20" s="88"/>
-      <c r="AZ20" s="88"/>
-      <c r="BA20" s="88"/>
-      <c r="BB20" s="88"/>
-      <c r="BC20" s="88"/>
-      <c r="BD20" s="88"/>
-      <c r="BE20" s="88"/>
-      <c r="BF20" s="88"/>
-      <c r="BG20" s="88"/>
-      <c r="BH20" s="88"/>
-      <c r="BI20" s="88"/>
-      <c r="BJ20" s="88"/>
-      <c r="BK20" s="88"/>
-      <c r="BL20" s="89"/>
+      <c r="AT20" s="96"/>
+      <c r="AU20" s="96"/>
+      <c r="AV20" s="96"/>
+      <c r="AW20" s="96"/>
+      <c r="AX20" s="96"/>
+      <c r="AY20" s="96"/>
+      <c r="AZ20" s="96"/>
+      <c r="BA20" s="96"/>
+      <c r="BB20" s="96"/>
+      <c r="BC20" s="96"/>
+      <c r="BD20" s="96"/>
+      <c r="BE20" s="96"/>
+      <c r="BF20" s="96"/>
+      <c r="BG20" s="96"/>
+      <c r="BH20" s="96"/>
+      <c r="BI20" s="96"/>
+      <c r="BJ20" s="96"/>
+      <c r="BK20" s="96"/>
+      <c r="BL20" s="97"/>
       <c r="BM20" s="18"/>
-      <c r="BO20" s="87" t="s">
+      <c r="BO20" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="BP20" s="88"/>
-      <c r="BQ20" s="88"/>
-      <c r="BR20" s="88"/>
-      <c r="BS20" s="88"/>
-      <c r="BT20" s="88"/>
-      <c r="BU20" s="88"/>
-      <c r="BV20" s="88"/>
-      <c r="BW20" s="88"/>
-      <c r="BX20" s="88"/>
-      <c r="BY20" s="88"/>
-      <c r="BZ20" s="89"/>
+      <c r="BP20" s="96"/>
+      <c r="BQ20" s="96"/>
+      <c r="BR20" s="96"/>
+      <c r="BS20" s="96"/>
+      <c r="BT20" s="96"/>
+      <c r="BU20" s="96"/>
+      <c r="BV20" s="96"/>
+      <c r="BW20" s="96"/>
+      <c r="BX20" s="96"/>
+      <c r="BY20" s="96"/>
+      <c r="BZ20" s="97"/>
     </row>
     <row r="21" spans="2:78" ht="4.5" customHeight="1">
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="51"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="52"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="60"/>
       <c r="U21" s="5"/>
-      <c r="W21" s="50"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="51"/>
-      <c r="Z21" s="51"/>
-      <c r="AA21" s="51"/>
-      <c r="AB21" s="51"/>
-      <c r="AC21" s="51"/>
-      <c r="AD21" s="51"/>
-      <c r="AE21" s="51"/>
-      <c r="AF21" s="51"/>
-      <c r="AG21" s="51"/>
-      <c r="AH21" s="51"/>
-      <c r="AI21" s="51"/>
-      <c r="AJ21" s="51"/>
-      <c r="AK21" s="51"/>
-      <c r="AL21" s="51"/>
-      <c r="AM21" s="51"/>
-      <c r="AN21" s="51"/>
-      <c r="AO21" s="51"/>
-      <c r="AP21" s="52"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="59"/>
+      <c r="Y21" s="59"/>
+      <c r="Z21" s="59"/>
+      <c r="AA21" s="59"/>
+      <c r="AB21" s="59"/>
+      <c r="AC21" s="59"/>
+      <c r="AD21" s="59"/>
+      <c r="AE21" s="59"/>
+      <c r="AF21" s="59"/>
+      <c r="AG21" s="59"/>
+      <c r="AH21" s="59"/>
+      <c r="AI21" s="59"/>
+      <c r="AJ21" s="59"/>
+      <c r="AK21" s="59"/>
+      <c r="AL21" s="59"/>
+      <c r="AM21" s="59"/>
+      <c r="AN21" s="59"/>
+      <c r="AO21" s="59"/>
+      <c r="AP21" s="60"/>
       <c r="AQ21" s="5"/>
-      <c r="AS21" s="50"/>
-      <c r="AT21" s="51"/>
-      <c r="AU21" s="51"/>
-      <c r="AV21" s="51"/>
-      <c r="AW21" s="51"/>
-      <c r="AX21" s="51"/>
-      <c r="AY21" s="51"/>
-      <c r="AZ21" s="51"/>
-      <c r="BA21" s="51"/>
-      <c r="BB21" s="51"/>
-      <c r="BC21" s="51"/>
-      <c r="BD21" s="51"/>
-      <c r="BE21" s="51"/>
-      <c r="BF21" s="51"/>
-      <c r="BG21" s="51"/>
-      <c r="BH21" s="51"/>
-      <c r="BI21" s="51"/>
-      <c r="BJ21" s="51"/>
-      <c r="BK21" s="51"/>
-      <c r="BL21" s="52"/>
+      <c r="AS21" s="58"/>
+      <c r="AT21" s="59"/>
+      <c r="AU21" s="59"/>
+      <c r="AV21" s="59"/>
+      <c r="AW21" s="59"/>
+      <c r="AX21" s="59"/>
+      <c r="AY21" s="59"/>
+      <c r="AZ21" s="59"/>
+      <c r="BA21" s="59"/>
+      <c r="BB21" s="59"/>
+      <c r="BC21" s="59"/>
+      <c r="BD21" s="59"/>
+      <c r="BE21" s="59"/>
+      <c r="BF21" s="59"/>
+      <c r="BG21" s="59"/>
+      <c r="BH21" s="59"/>
+      <c r="BI21" s="59"/>
+      <c r="BJ21" s="59"/>
+      <c r="BK21" s="59"/>
+      <c r="BL21" s="60"/>
       <c r="BM21" s="5"/>
-      <c r="BO21" s="123"/>
-      <c r="BP21" s="124"/>
-      <c r="BQ21" s="124"/>
-      <c r="BR21" s="124"/>
-      <c r="BS21" s="124"/>
-      <c r="BT21" s="124"/>
-      <c r="BU21" s="124"/>
-      <c r="BV21" s="124"/>
-      <c r="BW21" s="124"/>
-      <c r="BX21" s="124"/>
-      <c r="BY21" s="124"/>
-      <c r="BZ21" s="125"/>
+      <c r="BO21" s="125"/>
+      <c r="BP21" s="126"/>
+      <c r="BQ21" s="126"/>
+      <c r="BR21" s="126"/>
+      <c r="BS21" s="126"/>
+      <c r="BT21" s="126"/>
+      <c r="BU21" s="126"/>
+      <c r="BV21" s="126"/>
+      <c r="BW21" s="126"/>
+      <c r="BX21" s="126"/>
+      <c r="BY21" s="126"/>
+      <c r="BZ21" s="127"/>
     </row>
     <row r="22" spans="2:78" ht="12.75" customHeight="1">
-      <c r="B22" s="73" t="s">
+      <c r="B22" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="74"/>
-      <c r="T22" s="75"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="82"/>
+      <c r="S22" s="82"/>
+      <c r="T22" s="83"/>
       <c r="U22" s="19"/>
-      <c r="W22" s="73" t="s">
+      <c r="W22" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="X22" s="74"/>
-      <c r="Y22" s="74"/>
-      <c r="Z22" s="74"/>
-      <c r="AA22" s="74"/>
-      <c r="AB22" s="74"/>
-      <c r="AC22" s="74"/>
-      <c r="AD22" s="74"/>
-      <c r="AE22" s="74"/>
-      <c r="AF22" s="74"/>
-      <c r="AG22" s="74"/>
-      <c r="AH22" s="74"/>
-      <c r="AI22" s="74"/>
-      <c r="AJ22" s="74"/>
-      <c r="AK22" s="74"/>
-      <c r="AL22" s="74"/>
-      <c r="AM22" s="74"/>
-      <c r="AN22" s="74"/>
-      <c r="AO22" s="74"/>
-      <c r="AP22" s="75"/>
+      <c r="X22" s="82"/>
+      <c r="Y22" s="82"/>
+      <c r="Z22" s="82"/>
+      <c r="AA22" s="82"/>
+      <c r="AB22" s="82"/>
+      <c r="AC22" s="82"/>
+      <c r="AD22" s="82"/>
+      <c r="AE22" s="82"/>
+      <c r="AF22" s="82"/>
+      <c r="AG22" s="82"/>
+      <c r="AH22" s="82"/>
+      <c r="AI22" s="82"/>
+      <c r="AJ22" s="82"/>
+      <c r="AK22" s="82"/>
+      <c r="AL22" s="82"/>
+      <c r="AM22" s="82"/>
+      <c r="AN22" s="82"/>
+      <c r="AO22" s="82"/>
+      <c r="AP22" s="83"/>
       <c r="AQ22" s="19"/>
-      <c r="AS22" s="73" t="s">
+      <c r="AS22" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="AT22" s="74"/>
-      <c r="AU22" s="74"/>
-      <c r="AV22" s="74"/>
-      <c r="AW22" s="74"/>
-      <c r="AX22" s="74"/>
-      <c r="AY22" s="74"/>
-      <c r="AZ22" s="74"/>
-      <c r="BA22" s="74"/>
-      <c r="BB22" s="74"/>
-      <c r="BC22" s="74"/>
-      <c r="BD22" s="74"/>
-      <c r="BE22" s="74"/>
-      <c r="BF22" s="74"/>
-      <c r="BG22" s="74"/>
-      <c r="BH22" s="74"/>
-      <c r="BI22" s="74"/>
-      <c r="BJ22" s="74"/>
-      <c r="BK22" s="74"/>
-      <c r="BL22" s="75"/>
+      <c r="AT22" s="82"/>
+      <c r="AU22" s="82"/>
+      <c r="AV22" s="82"/>
+      <c r="AW22" s="82"/>
+      <c r="AX22" s="82"/>
+      <c r="AY22" s="82"/>
+      <c r="AZ22" s="82"/>
+      <c r="BA22" s="82"/>
+      <c r="BB22" s="82"/>
+      <c r="BC22" s="82"/>
+      <c r="BD22" s="82"/>
+      <c r="BE22" s="82"/>
+      <c r="BF22" s="82"/>
+      <c r="BG22" s="82"/>
+      <c r="BH22" s="82"/>
+      <c r="BI22" s="82"/>
+      <c r="BJ22" s="82"/>
+      <c r="BK22" s="82"/>
+      <c r="BL22" s="83"/>
       <c r="BM22" s="19"/>
-      <c r="BO22" s="73" t="s">
+      <c r="BO22" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="BP22" s="74"/>
-      <c r="BQ22" s="74"/>
-      <c r="BR22" s="74"/>
-      <c r="BS22" s="74"/>
-      <c r="BT22" s="74"/>
-      <c r="BU22" s="74"/>
-      <c r="BV22" s="74"/>
-      <c r="BW22" s="74"/>
-      <c r="BX22" s="74"/>
-      <c r="BY22" s="74"/>
-      <c r="BZ22" s="75"/>
+      <c r="BP22" s="82"/>
+      <c r="BQ22" s="82"/>
+      <c r="BR22" s="82"/>
+      <c r="BS22" s="82"/>
+      <c r="BT22" s="82"/>
+      <c r="BU22" s="82"/>
+      <c r="BV22" s="82"/>
+      <c r="BW22" s="82"/>
+      <c r="BX22" s="82"/>
+      <c r="BY22" s="82"/>
+      <c r="BZ22" s="83"/>
     </row>
     <row r="23" spans="2:78" ht="12.75" customHeight="1">
-      <c r="B23" s="76" t="s">
+      <c r="B23" s="84" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="77"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="77"/>
-      <c r="P23" s="77"/>
-      <c r="Q23" s="77"/>
-      <c r="R23" s="77"/>
-      <c r="S23" s="77"/>
-      <c r="T23" s="78"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="85"/>
+      <c r="N23" s="85"/>
+      <c r="O23" s="85"/>
+      <c r="P23" s="85"/>
+      <c r="Q23" s="85"/>
+      <c r="R23" s="85"/>
+      <c r="S23" s="85"/>
+      <c r="T23" s="86"/>
       <c r="U23" s="19"/>
-      <c r="W23" s="76" t="s">
+      <c r="W23" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="X23" s="77"/>
-      <c r="Y23" s="77"/>
-      <c r="Z23" s="77"/>
-      <c r="AA23" s="77"/>
-      <c r="AB23" s="77"/>
-      <c r="AC23" s="77"/>
-      <c r="AD23" s="77"/>
-      <c r="AE23" s="77"/>
-      <c r="AF23" s="77"/>
-      <c r="AG23" s="77"/>
-      <c r="AH23" s="77"/>
-      <c r="AI23" s="77"/>
-      <c r="AJ23" s="77"/>
-      <c r="AK23" s="77"/>
-      <c r="AL23" s="77"/>
-      <c r="AM23" s="77"/>
-      <c r="AN23" s="77"/>
-      <c r="AO23" s="77"/>
-      <c r="AP23" s="78"/>
+      <c r="X23" s="85"/>
+      <c r="Y23" s="85"/>
+      <c r="Z23" s="85"/>
+      <c r="AA23" s="85"/>
+      <c r="AB23" s="85"/>
+      <c r="AC23" s="85"/>
+      <c r="AD23" s="85"/>
+      <c r="AE23" s="85"/>
+      <c r="AF23" s="85"/>
+      <c r="AG23" s="85"/>
+      <c r="AH23" s="85"/>
+      <c r="AI23" s="85"/>
+      <c r="AJ23" s="85"/>
+      <c r="AK23" s="85"/>
+      <c r="AL23" s="85"/>
+      <c r="AM23" s="85"/>
+      <c r="AN23" s="85"/>
+      <c r="AO23" s="85"/>
+      <c r="AP23" s="86"/>
       <c r="AQ23" s="19"/>
-      <c r="AS23" s="76" t="s">
+      <c r="AS23" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="AT23" s="77"/>
-      <c r="AU23" s="77"/>
-      <c r="AV23" s="77"/>
-      <c r="AW23" s="77"/>
-      <c r="AX23" s="77"/>
-      <c r="AY23" s="77"/>
-      <c r="AZ23" s="77"/>
-      <c r="BA23" s="77"/>
-      <c r="BB23" s="77"/>
-      <c r="BC23" s="77"/>
-      <c r="BD23" s="77"/>
-      <c r="BE23" s="77"/>
-      <c r="BF23" s="77"/>
-      <c r="BG23" s="77"/>
-      <c r="BH23" s="77"/>
-      <c r="BI23" s="77"/>
-      <c r="BJ23" s="77"/>
-      <c r="BK23" s="77"/>
-      <c r="BL23" s="78"/>
+      <c r="AT23" s="85"/>
+      <c r="AU23" s="85"/>
+      <c r="AV23" s="85"/>
+      <c r="AW23" s="85"/>
+      <c r="AX23" s="85"/>
+      <c r="AY23" s="85"/>
+      <c r="AZ23" s="85"/>
+      <c r="BA23" s="85"/>
+      <c r="BB23" s="85"/>
+      <c r="BC23" s="85"/>
+      <c r="BD23" s="85"/>
+      <c r="BE23" s="85"/>
+      <c r="BF23" s="85"/>
+      <c r="BG23" s="85"/>
+      <c r="BH23" s="85"/>
+      <c r="BI23" s="85"/>
+      <c r="BJ23" s="85"/>
+      <c r="BK23" s="85"/>
+      <c r="BL23" s="86"/>
       <c r="BM23" s="19"/>
-      <c r="BO23" s="76" t="s">
+      <c r="BO23" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="BP23" s="77"/>
-      <c r="BQ23" s="77"/>
-      <c r="BR23" s="77"/>
-      <c r="BS23" s="77"/>
-      <c r="BT23" s="77"/>
-      <c r="BU23" s="77"/>
-      <c r="BV23" s="77"/>
-      <c r="BW23" s="77"/>
-      <c r="BX23" s="77"/>
-      <c r="BY23" s="77"/>
-      <c r="BZ23" s="78"/>
+      <c r="BP23" s="85"/>
+      <c r="BQ23" s="85"/>
+      <c r="BR23" s="85"/>
+      <c r="BS23" s="85"/>
+      <c r="BT23" s="85"/>
+      <c r="BU23" s="85"/>
+      <c r="BV23" s="85"/>
+      <c r="BW23" s="85"/>
+      <c r="BX23" s="85"/>
+      <c r="BY23" s="85"/>
+      <c r="BZ23" s="86"/>
     </row>
     <row r="24" spans="2:78" ht="16.5" customHeight="1">
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
-      <c r="J24" s="77"/>
-      <c r="K24" s="77"/>
-      <c r="L24" s="77"/>
-      <c r="M24" s="77"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="77"/>
-      <c r="P24" s="77"/>
-      <c r="Q24" s="77"/>
-      <c r="R24" s="77"/>
-      <c r="S24" s="77"/>
-      <c r="T24" s="78"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="85"/>
+      <c r="M24" s="85"/>
+      <c r="N24" s="85"/>
+      <c r="O24" s="85"/>
+      <c r="P24" s="85"/>
+      <c r="Q24" s="85"/>
+      <c r="R24" s="85"/>
+      <c r="S24" s="85"/>
+      <c r="T24" s="86"/>
       <c r="U24" s="5"/>
-      <c r="W24" s="76" t="s">
+      <c r="W24" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="X24" s="77"/>
-      <c r="Y24" s="77"/>
-      <c r="Z24" s="77"/>
-      <c r="AA24" s="77"/>
-      <c r="AB24" s="77"/>
-      <c r="AC24" s="77"/>
-      <c r="AD24" s="77"/>
-      <c r="AE24" s="77"/>
-      <c r="AF24" s="77"/>
-      <c r="AG24" s="77"/>
-      <c r="AH24" s="77"/>
-      <c r="AI24" s="77"/>
-      <c r="AJ24" s="77"/>
-      <c r="AK24" s="77"/>
-      <c r="AL24" s="77"/>
-      <c r="AM24" s="77"/>
-      <c r="AN24" s="77"/>
-      <c r="AO24" s="77"/>
-      <c r="AP24" s="78"/>
+      <c r="X24" s="85"/>
+      <c r="Y24" s="85"/>
+      <c r="Z24" s="85"/>
+      <c r="AA24" s="85"/>
+      <c r="AB24" s="85"/>
+      <c r="AC24" s="85"/>
+      <c r="AD24" s="85"/>
+      <c r="AE24" s="85"/>
+      <c r="AF24" s="85"/>
+      <c r="AG24" s="85"/>
+      <c r="AH24" s="85"/>
+      <c r="AI24" s="85"/>
+      <c r="AJ24" s="85"/>
+      <c r="AK24" s="85"/>
+      <c r="AL24" s="85"/>
+      <c r="AM24" s="85"/>
+      <c r="AN24" s="85"/>
+      <c r="AO24" s="85"/>
+      <c r="AP24" s="86"/>
       <c r="AQ24" s="5"/>
-      <c r="AS24" s="76" t="s">
+      <c r="AS24" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="AT24" s="77"/>
-      <c r="AU24" s="77"/>
-      <c r="AV24" s="77"/>
-      <c r="AW24" s="77"/>
-      <c r="AX24" s="77"/>
-      <c r="AY24" s="77"/>
-      <c r="AZ24" s="77"/>
-      <c r="BA24" s="77"/>
-      <c r="BB24" s="77"/>
-      <c r="BC24" s="77"/>
-      <c r="BD24" s="77"/>
-      <c r="BE24" s="77"/>
-      <c r="BF24" s="77"/>
-      <c r="BG24" s="77"/>
-      <c r="BH24" s="77"/>
-      <c r="BI24" s="77"/>
-      <c r="BJ24" s="77"/>
-      <c r="BK24" s="77"/>
-      <c r="BL24" s="78"/>
+      <c r="AT24" s="85"/>
+      <c r="AU24" s="85"/>
+      <c r="AV24" s="85"/>
+      <c r="AW24" s="85"/>
+      <c r="AX24" s="85"/>
+      <c r="AY24" s="85"/>
+      <c r="AZ24" s="85"/>
+      <c r="BA24" s="85"/>
+      <c r="BB24" s="85"/>
+      <c r="BC24" s="85"/>
+      <c r="BD24" s="85"/>
+      <c r="BE24" s="85"/>
+      <c r="BF24" s="85"/>
+      <c r="BG24" s="85"/>
+      <c r="BH24" s="85"/>
+      <c r="BI24" s="85"/>
+      <c r="BJ24" s="85"/>
+      <c r="BK24" s="85"/>
+      <c r="BL24" s="86"/>
       <c r="BM24" s="5"/>
-      <c r="BO24" s="76" t="s">
+      <c r="BO24" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="BP24" s="77"/>
-      <c r="BQ24" s="77"/>
-      <c r="BR24" s="77"/>
-      <c r="BS24" s="77"/>
-      <c r="BT24" s="77"/>
-      <c r="BU24" s="77"/>
-      <c r="BV24" s="77"/>
-      <c r="BW24" s="77"/>
-      <c r="BX24" s="77"/>
-      <c r="BY24" s="77"/>
-      <c r="BZ24" s="78"/>
+      <c r="BP24" s="85"/>
+      <c r="BQ24" s="85"/>
+      <c r="BR24" s="85"/>
+      <c r="BS24" s="85"/>
+      <c r="BT24" s="85"/>
+      <c r="BU24" s="85"/>
+      <c r="BV24" s="85"/>
+      <c r="BW24" s="85"/>
+      <c r="BX24" s="85"/>
+      <c r="BY24" s="85"/>
+      <c r="BZ24" s="86"/>
     </row>
     <row r="25" spans="2:78" ht="12.75" customHeight="1">
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="77"/>
-      <c r="D25" s="77"/>
-      <c r="E25" s="77"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="77"/>
-      <c r="J25" s="77"/>
-      <c r="K25" s="77"/>
-      <c r="L25" s="77"/>
-      <c r="M25" s="77"/>
-      <c r="N25" s="77"/>
-      <c r="O25" s="77"/>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="77"/>
-      <c r="R25" s="77"/>
-      <c r="S25" s="80" t="s">
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="85"/>
+      <c r="N25" s="85"/>
+      <c r="O25" s="85"/>
+      <c r="P25" s="85"/>
+      <c r="Q25" s="85"/>
+      <c r="R25" s="85"/>
+      <c r="S25" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="T25" s="81"/>
+      <c r="T25" s="89"/>
       <c r="U25" s="20"/>
-      <c r="W25" s="76" t="s">
+      <c r="W25" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="X25" s="77"/>
-      <c r="Y25" s="77"/>
-      <c r="Z25" s="77"/>
-      <c r="AA25" s="77"/>
-      <c r="AB25" s="77"/>
-      <c r="AC25" s="77"/>
-      <c r="AD25" s="77"/>
-      <c r="AE25" s="77"/>
-      <c r="AF25" s="77"/>
-      <c r="AG25" s="77"/>
-      <c r="AH25" s="77"/>
-      <c r="AI25" s="77"/>
-      <c r="AJ25" s="77"/>
-      <c r="AK25" s="77"/>
-      <c r="AL25" s="77"/>
-      <c r="AM25" s="77"/>
-      <c r="AN25" s="77"/>
-      <c r="AO25" s="63"/>
-      <c r="AP25" s="64"/>
+      <c r="X25" s="85"/>
+      <c r="Y25" s="85"/>
+      <c r="Z25" s="85"/>
+      <c r="AA25" s="85"/>
+      <c r="AB25" s="85"/>
+      <c r="AC25" s="85"/>
+      <c r="AD25" s="85"/>
+      <c r="AE25" s="85"/>
+      <c r="AF25" s="85"/>
+      <c r="AG25" s="85"/>
+      <c r="AH25" s="85"/>
+      <c r="AI25" s="85"/>
+      <c r="AJ25" s="85"/>
+      <c r="AK25" s="85"/>
+      <c r="AL25" s="85"/>
+      <c r="AM25" s="85"/>
+      <c r="AN25" s="85"/>
+      <c r="AO25" s="71"/>
+      <c r="AP25" s="72"/>
       <c r="AQ25" s="21"/>
-      <c r="AS25" s="178" t="s">
+      <c r="AS25" s="180" t="s">
         <v>90</v>
       </c>
-      <c r="AT25" s="179"/>
-      <c r="AU25" s="179"/>
-      <c r="AV25" s="179"/>
-      <c r="AW25" s="179"/>
-      <c r="AX25" s="179"/>
-      <c r="AY25" s="179"/>
-      <c r="AZ25" s="179"/>
-      <c r="BA25" s="179"/>
-      <c r="BB25" s="179"/>
-      <c r="BC25" s="179"/>
-      <c r="BD25" s="179"/>
-      <c r="BE25" s="179"/>
-      <c r="BF25" s="179"/>
-      <c r="BG25" s="179"/>
-      <c r="BH25" s="179"/>
-      <c r="BI25" s="179"/>
-      <c r="BJ25" s="179"/>
-      <c r="BK25" s="80" t="s">
+      <c r="AT25" s="181"/>
+      <c r="AU25" s="181"/>
+      <c r="AV25" s="181"/>
+      <c r="AW25" s="181"/>
+      <c r="AX25" s="181"/>
+      <c r="AY25" s="181"/>
+      <c r="AZ25" s="181"/>
+      <c r="BA25" s="181"/>
+      <c r="BB25" s="181"/>
+      <c r="BC25" s="181"/>
+      <c r="BD25" s="181"/>
+      <c r="BE25" s="181"/>
+      <c r="BF25" s="181"/>
+      <c r="BG25" s="181"/>
+      <c r="BH25" s="181"/>
+      <c r="BI25" s="181"/>
+      <c r="BJ25" s="181"/>
+      <c r="BK25" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="BL25" s="81"/>
+      <c r="BL25" s="89"/>
       <c r="BM25" s="20"/>
-      <c r="BO25" s="76" t="s">
+      <c r="BO25" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="BP25" s="77"/>
-      <c r="BQ25" s="77"/>
-      <c r="BR25" s="77"/>
-      <c r="BS25" s="77"/>
-      <c r="BT25" s="77"/>
-      <c r="BU25" s="77"/>
-      <c r="BV25" s="77"/>
-      <c r="BW25" s="77"/>
-      <c r="BX25" s="77"/>
-      <c r="BY25" s="80" t="s">
+      <c r="BP25" s="85"/>
+      <c r="BQ25" s="85"/>
+      <c r="BR25" s="85"/>
+      <c r="BS25" s="85"/>
+      <c r="BT25" s="85"/>
+      <c r="BU25" s="85"/>
+      <c r="BV25" s="85"/>
+      <c r="BW25" s="85"/>
+      <c r="BX25" s="85"/>
+      <c r="BY25" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="BZ25" s="81"/>
+      <c r="BZ25" s="89"/>
     </row>
     <row r="26" spans="2:78" ht="12.75" customHeight="1">
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
       <c r="G26" s="29"/>
-      <c r="H26" s="202" t="s">
+      <c r="H26" s="204" t="s">
         <v>82</v>
       </c>
-      <c r="I26" s="202"/>
-      <c r="J26" s="202"/>
-      <c r="K26" s="202"/>
-      <c r="L26" s="202"/>
-      <c r="M26" s="202"/>
-      <c r="N26" s="202"/>
-      <c r="O26" s="202"/>
-      <c r="P26" s="202"/>
-      <c r="Q26" s="202"/>
-      <c r="R26" s="202"/>
-      <c r="S26" s="80"/>
-      <c r="T26" s="81"/>
+      <c r="I26" s="204"/>
+      <c r="J26" s="204"/>
+      <c r="K26" s="204"/>
+      <c r="L26" s="204"/>
+      <c r="M26" s="204"/>
+      <c r="N26" s="204"/>
+      <c r="O26" s="204"/>
+      <c r="P26" s="204"/>
+      <c r="Q26" s="204"/>
+      <c r="R26" s="204"/>
+      <c r="S26" s="88"/>
+      <c r="T26" s="89"/>
       <c r="U26" s="20"/>
-      <c r="W26" s="76" t="s">
+      <c r="W26" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="X26" s="77"/>
-      <c r="Y26" s="77"/>
-      <c r="Z26" s="77"/>
-      <c r="AA26" s="77"/>
+      <c r="X26" s="85"/>
+      <c r="Y26" s="85"/>
+      <c r="Z26" s="85"/>
+      <c r="AA26" s="85"/>
       <c r="AB26" s="29"/>
-      <c r="AC26" s="202" t="s">
+      <c r="AC26" s="204" t="s">
         <v>82</v>
       </c>
-      <c r="AD26" s="202"/>
-      <c r="AE26" s="202"/>
-      <c r="AF26" s="202"/>
-      <c r="AG26" s="202"/>
-      <c r="AH26" s="202"/>
-      <c r="AI26" s="202"/>
-      <c r="AJ26" s="202"/>
-      <c r="AK26" s="202"/>
-      <c r="AL26" s="202"/>
-      <c r="AM26" s="202"/>
+      <c r="AD26" s="204"/>
+      <c r="AE26" s="204"/>
+      <c r="AF26" s="204"/>
+      <c r="AG26" s="204"/>
+      <c r="AH26" s="204"/>
+      <c r="AI26" s="204"/>
+      <c r="AJ26" s="204"/>
+      <c r="AK26" s="204"/>
+      <c r="AL26" s="204"/>
+      <c r="AM26" s="204"/>
       <c r="AN26" s="29"/>
-      <c r="AO26" s="63"/>
-      <c r="AP26" s="64"/>
+      <c r="AO26" s="71"/>
+      <c r="AP26" s="72"/>
       <c r="AQ26" s="21"/>
-      <c r="AS26" s="76" t="s">
+      <c r="AS26" s="84" t="s">
         <v>89</v>
       </c>
-      <c r="AT26" s="77"/>
-      <c r="AU26" s="77"/>
-      <c r="AV26" s="77"/>
-      <c r="AW26" s="77"/>
+      <c r="AT26" s="85"/>
+      <c r="AU26" s="85"/>
+      <c r="AV26" s="85"/>
+      <c r="AW26" s="85"/>
       <c r="AX26" s="29"/>
       <c r="AY26" s="29"/>
-      <c r="AZ26" s="202" t="s">
+      <c r="AZ26" s="204" t="s">
         <v>82</v>
       </c>
-      <c r="BA26" s="202"/>
-      <c r="BB26" s="202"/>
-      <c r="BC26" s="202"/>
-      <c r="BD26" s="202"/>
-      <c r="BE26" s="202"/>
-      <c r="BF26" s="202"/>
-      <c r="BG26" s="202"/>
-      <c r="BH26" s="202"/>
-      <c r="BI26" s="202"/>
-      <c r="BJ26" s="202"/>
-      <c r="BK26" s="80"/>
-      <c r="BL26" s="81"/>
+      <c r="BA26" s="204"/>
+      <c r="BB26" s="204"/>
+      <c r="BC26" s="204"/>
+      <c r="BD26" s="204"/>
+      <c r="BE26" s="204"/>
+      <c r="BF26" s="204"/>
+      <c r="BG26" s="204"/>
+      <c r="BH26" s="204"/>
+      <c r="BI26" s="204"/>
+      <c r="BJ26" s="204"/>
+      <c r="BK26" s="88"/>
+      <c r="BL26" s="89"/>
       <c r="BM26" s="20"/>
       <c r="BO26" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="BP26" s="201" t="s">
+      <c r="BP26" s="203" t="s">
         <v>82</v>
       </c>
-      <c r="BQ26" s="201"/>
-      <c r="BR26" s="201"/>
-      <c r="BS26" s="201"/>
-      <c r="BT26" s="201"/>
-      <c r="BU26" s="201"/>
-      <c r="BV26" s="201"/>
-      <c r="BW26" s="201"/>
+      <c r="BQ26" s="203"/>
+      <c r="BR26" s="203"/>
+      <c r="BS26" s="203"/>
+      <c r="BT26" s="203"/>
+      <c r="BU26" s="203"/>
+      <c r="BV26" s="203"/>
+      <c r="BW26" s="203"/>
       <c r="BX26" s="33"/>
-      <c r="BY26" s="80"/>
-      <c r="BZ26" s="81"/>
+      <c r="BY26" s="88"/>
+      <c r="BZ26" s="89"/>
     </row>
     <row r="27" spans="2:78" ht="6" customHeight="1">
-      <c r="B27" s="196"/>
-      <c r="C27" s="197"/>
-      <c r="D27" s="197"/>
-      <c r="E27" s="197"/>
-      <c r="F27" s="197"/>
-      <c r="G27" s="197"/>
-      <c r="H27" s="197"/>
-      <c r="I27" s="197"/>
-      <c r="J27" s="197"/>
-      <c r="K27" s="197"/>
-      <c r="L27" s="197"/>
-      <c r="M27" s="197"/>
-      <c r="N27" s="197"/>
-      <c r="O27" s="197"/>
-      <c r="P27" s="197"/>
-      <c r="Q27" s="197"/>
-      <c r="R27" s="197"/>
-      <c r="S27" s="82"/>
-      <c r="T27" s="83"/>
+      <c r="B27" s="198"/>
+      <c r="C27" s="199"/>
+      <c r="D27" s="199"/>
+      <c r="E27" s="199"/>
+      <c r="F27" s="199"/>
+      <c r="G27" s="199"/>
+      <c r="H27" s="199"/>
+      <c r="I27" s="199"/>
+      <c r="J27" s="199"/>
+      <c r="K27" s="199"/>
+      <c r="L27" s="199"/>
+      <c r="M27" s="199"/>
+      <c r="N27" s="199"/>
+      <c r="O27" s="199"/>
+      <c r="P27" s="199"/>
+      <c r="Q27" s="199"/>
+      <c r="R27" s="199"/>
+      <c r="S27" s="90"/>
+      <c r="T27" s="91"/>
       <c r="U27" s="20"/>
       <c r="W27" s="23"/>
       <c r="X27" s="22"/>
@@ -5281,8 +5278,8 @@
       <c r="AL27" s="24"/>
       <c r="AM27" s="24"/>
       <c r="AN27" s="24"/>
-      <c r="AO27" s="65"/>
-      <c r="AP27" s="66"/>
+      <c r="AO27" s="73"/>
+      <c r="AP27" s="74"/>
       <c r="AQ27" s="21"/>
       <c r="AS27" s="23"/>
       <c r="AT27" s="22"/>
@@ -5302,8 +5299,8 @@
       <c r="BH27" s="24"/>
       <c r="BI27" s="24"/>
       <c r="BJ27" s="24"/>
-      <c r="BK27" s="82"/>
-      <c r="BL27" s="83"/>
+      <c r="BK27" s="90"/>
+      <c r="BL27" s="91"/>
       <c r="BM27" s="20"/>
       <c r="BO27" s="30"/>
       <c r="BP27" s="31"/>
@@ -5315,83 +5312,83 @@
       <c r="BV27" s="31"/>
       <c r="BW27" s="31"/>
       <c r="BX27" s="31"/>
-      <c r="BY27" s="82"/>
-      <c r="BZ27" s="83"/>
+      <c r="BY27" s="90"/>
+      <c r="BZ27" s="91"/>
     </row>
     <row r="28" spans="2:78" ht="13.5" customHeight="1">
-      <c r="B28" s="189" t="s">
+      <c r="B28" s="191" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="189"/>
-      <c r="D28" s="189"/>
-      <c r="E28" s="189"/>
-      <c r="F28" s="189"/>
-      <c r="G28" s="189"/>
-      <c r="H28" s="189"/>
-      <c r="I28" s="189"/>
-      <c r="J28" s="189"/>
-      <c r="K28" s="189"/>
-      <c r="L28" s="189"/>
-      <c r="M28" s="190"/>
-      <c r="N28" s="44" t="s">
+      <c r="C28" s="191"/>
+      <c r="D28" s="191"/>
+      <c r="E28" s="191"/>
+      <c r="F28" s="191"/>
+      <c r="G28" s="191"/>
+      <c r="H28" s="191"/>
+      <c r="I28" s="191"/>
+      <c r="J28" s="191"/>
+      <c r="K28" s="191"/>
+      <c r="L28" s="191"/>
+      <c r="M28" s="192"/>
+      <c r="N28" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="O28" s="47"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="48"/>
-      <c r="R28" s="48"/>
-      <c r="S28" s="48"/>
-      <c r="T28" s="49"/>
+      <c r="O28" s="55"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="57"/>
       <c r="U28" s="5"/>
-      <c r="W28" s="60" t="s">
+      <c r="W28" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="X28" s="61"/>
-      <c r="Y28" s="61"/>
-      <c r="Z28" s="61"/>
-      <c r="AA28" s="61"/>
-      <c r="AB28" s="61"/>
-      <c r="AC28" s="61"/>
-      <c r="AD28" s="61"/>
-      <c r="AE28" s="61"/>
-      <c r="AF28" s="61"/>
-      <c r="AG28" s="61"/>
-      <c r="AH28" s="61"/>
-      <c r="AI28" s="62"/>
-      <c r="AJ28" s="44" t="s">
+      <c r="X28" s="69"/>
+      <c r="Y28" s="69"/>
+      <c r="Z28" s="69"/>
+      <c r="AA28" s="69"/>
+      <c r="AB28" s="69"/>
+      <c r="AC28" s="69"/>
+      <c r="AD28" s="69"/>
+      <c r="AE28" s="69"/>
+      <c r="AF28" s="69"/>
+      <c r="AG28" s="69"/>
+      <c r="AH28" s="69"/>
+      <c r="AI28" s="70"/>
+      <c r="AJ28" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="AK28" s="47"/>
-      <c r="AL28" s="48"/>
-      <c r="AM28" s="48"/>
-      <c r="AN28" s="48"/>
-      <c r="AO28" s="48"/>
-      <c r="AP28" s="49"/>
+      <c r="AK28" s="55"/>
+      <c r="AL28" s="56"/>
+      <c r="AM28" s="56"/>
+      <c r="AN28" s="56"/>
+      <c r="AO28" s="56"/>
+      <c r="AP28" s="57"/>
       <c r="AQ28" s="5"/>
-      <c r="AS28" s="144" t="s">
+      <c r="AS28" s="146" t="s">
         <v>46</v>
       </c>
-      <c r="AT28" s="145"/>
-      <c r="AU28" s="145"/>
-      <c r="AV28" s="145"/>
-      <c r="AW28" s="145"/>
-      <c r="AX28" s="145"/>
-      <c r="AY28" s="145"/>
-      <c r="AZ28" s="145"/>
-      <c r="BA28" s="145"/>
-      <c r="BB28" s="145"/>
-      <c r="BC28" s="145"/>
-      <c r="BD28" s="145"/>
-      <c r="BE28" s="146"/>
-      <c r="BF28" s="44" t="s">
+      <c r="AT28" s="147"/>
+      <c r="AU28" s="147"/>
+      <c r="AV28" s="147"/>
+      <c r="AW28" s="147"/>
+      <c r="AX28" s="147"/>
+      <c r="AY28" s="147"/>
+      <c r="AZ28" s="147"/>
+      <c r="BA28" s="147"/>
+      <c r="BB28" s="147"/>
+      <c r="BC28" s="147"/>
+      <c r="BD28" s="147"/>
+      <c r="BE28" s="148"/>
+      <c r="BF28" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="BG28" s="47"/>
-      <c r="BH28" s="48"/>
-      <c r="BI28" s="48"/>
-      <c r="BJ28" s="48"/>
-      <c r="BK28" s="48"/>
-      <c r="BL28" s="49"/>
+      <c r="BG28" s="55"/>
+      <c r="BH28" s="56"/>
+      <c r="BI28" s="56"/>
+      <c r="BJ28" s="56"/>
+      <c r="BK28" s="56"/>
+      <c r="BL28" s="57"/>
       <c r="BM28" s="5"/>
       <c r="BO28" s="25" t="s">
         <v>31</v>
@@ -5421,76 +5418,76 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="50"/>
-      <c r="P29" s="51"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="51"/>
-      <c r="S29" s="51"/>
-      <c r="T29" s="52"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
+      <c r="S29" s="59"/>
+      <c r="T29" s="60"/>
       <c r="U29" s="5"/>
-      <c r="W29" s="147" t="s">
+      <c r="W29" s="149" t="s">
         <v>45</v>
       </c>
-      <c r="X29" s="148"/>
-      <c r="Y29" s="148"/>
-      <c r="Z29" s="149"/>
-      <c r="AA29" s="90" t="s">
+      <c r="X29" s="150"/>
+      <c r="Y29" s="150"/>
+      <c r="Z29" s="151"/>
+      <c r="AA29" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="AB29" s="91"/>
-      <c r="AC29" s="91"/>
-      <c r="AD29" s="91"/>
-      <c r="AE29" s="91"/>
-      <c r="AF29" s="91"/>
-      <c r="AG29" s="91"/>
-      <c r="AH29" s="91"/>
-      <c r="AI29" s="92"/>
-      <c r="AJ29" s="45"/>
-      <c r="AK29" s="50"/>
-      <c r="AL29" s="51"/>
-      <c r="AM29" s="51"/>
-      <c r="AN29" s="51"/>
-      <c r="AO29" s="51"/>
-      <c r="AP29" s="52"/>
+      <c r="AB29" s="99"/>
+      <c r="AC29" s="99"/>
+      <c r="AD29" s="99"/>
+      <c r="AE29" s="99"/>
+      <c r="AF29" s="99"/>
+      <c r="AG29" s="99"/>
+      <c r="AH29" s="99"/>
+      <c r="AI29" s="100"/>
+      <c r="AJ29" s="53"/>
+      <c r="AK29" s="58"/>
+      <c r="AL29" s="59"/>
+      <c r="AM29" s="59"/>
+      <c r="AN29" s="59"/>
+      <c r="AO29" s="59"/>
+      <c r="AP29" s="60"/>
       <c r="AQ29" s="5"/>
-      <c r="AS29" s="147" t="s">
-        <v>96</v>
-      </c>
-      <c r="AT29" s="148"/>
-      <c r="AU29" s="148"/>
-      <c r="AV29" s="148"/>
-      <c r="AW29" s="148"/>
-      <c r="AX29" s="148"/>
-      <c r="AY29" s="148"/>
-      <c r="AZ29" s="148"/>
-      <c r="BA29" s="148"/>
-      <c r="BB29" s="148"/>
-      <c r="BC29" s="148"/>
-      <c r="BD29" s="148"/>
-      <c r="BE29" s="149"/>
-      <c r="BF29" s="45"/>
-      <c r="BG29" s="50"/>
-      <c r="BH29" s="51"/>
-      <c r="BI29" s="51"/>
-      <c r="BJ29" s="51"/>
-      <c r="BK29" s="51"/>
-      <c r="BL29" s="52"/>
+      <c r="AS29" s="149" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT29" s="150"/>
+      <c r="AU29" s="150"/>
+      <c r="AV29" s="150"/>
+      <c r="AW29" s="150"/>
+      <c r="AX29" s="150"/>
+      <c r="AY29" s="150"/>
+      <c r="AZ29" s="150"/>
+      <c r="BA29" s="150"/>
+      <c r="BB29" s="150"/>
+      <c r="BC29" s="150"/>
+      <c r="BD29" s="150"/>
+      <c r="BE29" s="151"/>
+      <c r="BF29" s="53"/>
+      <c r="BG29" s="58"/>
+      <c r="BH29" s="59"/>
+      <c r="BI29" s="59"/>
+      <c r="BJ29" s="59"/>
+      <c r="BK29" s="59"/>
+      <c r="BL29" s="60"/>
       <c r="BM29" s="5"/>
-      <c r="BO29" s="56" t="s">
+      <c r="BO29" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="BP29" s="57"/>
-      <c r="BQ29" s="57"/>
-      <c r="BR29" s="57"/>
-      <c r="BS29" s="57"/>
-      <c r="BT29" s="57"/>
-      <c r="BU29" s="57"/>
-      <c r="BV29" s="57"/>
-      <c r="BW29" s="57"/>
-      <c r="BX29" s="57"/>
-      <c r="BY29" s="57"/>
-      <c r="BZ29" s="58"/>
+      <c r="BP29" s="65"/>
+      <c r="BQ29" s="65"/>
+      <c r="BR29" s="65"/>
+      <c r="BS29" s="65"/>
+      <c r="BT29" s="65"/>
+      <c r="BU29" s="65"/>
+      <c r="BV29" s="65"/>
+      <c r="BW29" s="65"/>
+      <c r="BX29" s="65"/>
+      <c r="BY29" s="65"/>
+      <c r="BZ29" s="66"/>
     </row>
     <row r="30" spans="2:78" ht="8.25" customHeight="1">
       <c r="B30" s="3"/>
@@ -5505,70 +5502,70 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="50"/>
-      <c r="P30" s="51"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="51"/>
-      <c r="S30" s="51"/>
-      <c r="T30" s="52"/>
+      <c r="N30" s="53"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="59"/>
+      <c r="R30" s="59"/>
+      <c r="S30" s="59"/>
+      <c r="T30" s="60"/>
       <c r="U30" s="5"/>
-      <c r="W30" s="198"/>
-      <c r="X30" s="199"/>
-      <c r="Y30" s="199"/>
-      <c r="Z30" s="200"/>
-      <c r="AA30" s="93"/>
-      <c r="AB30" s="94"/>
-      <c r="AC30" s="94"/>
-      <c r="AD30" s="94"/>
-      <c r="AE30" s="94"/>
-      <c r="AF30" s="94"/>
-      <c r="AG30" s="94"/>
-      <c r="AH30" s="94"/>
-      <c r="AI30" s="95"/>
-      <c r="AJ30" s="45"/>
-      <c r="AK30" s="50"/>
-      <c r="AL30" s="51"/>
-      <c r="AM30" s="51"/>
-      <c r="AN30" s="51"/>
-      <c r="AO30" s="51"/>
-      <c r="AP30" s="52"/>
+      <c r="W30" s="200"/>
+      <c r="X30" s="201"/>
+      <c r="Y30" s="201"/>
+      <c r="Z30" s="202"/>
+      <c r="AA30" s="101"/>
+      <c r="AB30" s="102"/>
+      <c r="AC30" s="102"/>
+      <c r="AD30" s="102"/>
+      <c r="AE30" s="102"/>
+      <c r="AF30" s="102"/>
+      <c r="AG30" s="102"/>
+      <c r="AH30" s="102"/>
+      <c r="AI30" s="103"/>
+      <c r="AJ30" s="53"/>
+      <c r="AK30" s="58"/>
+      <c r="AL30" s="59"/>
+      <c r="AM30" s="59"/>
+      <c r="AN30" s="59"/>
+      <c r="AO30" s="59"/>
+      <c r="AP30" s="60"/>
       <c r="AQ30" s="5"/>
-      <c r="AS30" s="73" t="s">
+      <c r="AS30" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="AT30" s="74"/>
-      <c r="AU30" s="74"/>
-      <c r="AV30" s="74"/>
-      <c r="AW30" s="74"/>
-      <c r="AX30" s="74"/>
-      <c r="AY30" s="74"/>
-      <c r="AZ30" s="74"/>
-      <c r="BA30" s="74"/>
-      <c r="BB30" s="74"/>
-      <c r="BC30" s="74"/>
-      <c r="BD30" s="74"/>
-      <c r="BE30" s="75"/>
-      <c r="BF30" s="45"/>
-      <c r="BG30" s="50"/>
-      <c r="BH30" s="51"/>
-      <c r="BI30" s="51"/>
-      <c r="BJ30" s="51"/>
-      <c r="BK30" s="51"/>
-      <c r="BL30" s="52"/>
+      <c r="AT30" s="82"/>
+      <c r="AU30" s="82"/>
+      <c r="AV30" s="82"/>
+      <c r="AW30" s="82"/>
+      <c r="AX30" s="82"/>
+      <c r="AY30" s="82"/>
+      <c r="AZ30" s="82"/>
+      <c r="BA30" s="82"/>
+      <c r="BB30" s="82"/>
+      <c r="BC30" s="82"/>
+      <c r="BD30" s="82"/>
+      <c r="BE30" s="83"/>
+      <c r="BF30" s="53"/>
+      <c r="BG30" s="58"/>
+      <c r="BH30" s="59"/>
+      <c r="BI30" s="59"/>
+      <c r="BJ30" s="59"/>
+      <c r="BK30" s="59"/>
+      <c r="BL30" s="60"/>
       <c r="BM30" s="5"/>
-      <c r="BO30" s="59"/>
-      <c r="BP30" s="57"/>
-      <c r="BQ30" s="57"/>
-      <c r="BR30" s="57"/>
-      <c r="BS30" s="57"/>
-      <c r="BT30" s="57"/>
-      <c r="BU30" s="57"/>
-      <c r="BV30" s="57"/>
-      <c r="BW30" s="57"/>
-      <c r="BX30" s="57"/>
-      <c r="BY30" s="57"/>
-      <c r="BZ30" s="58"/>
+      <c r="BO30" s="67"/>
+      <c r="BP30" s="65"/>
+      <c r="BQ30" s="65"/>
+      <c r="BR30" s="65"/>
+      <c r="BS30" s="65"/>
+      <c r="BT30" s="65"/>
+      <c r="BU30" s="65"/>
+      <c r="BV30" s="65"/>
+      <c r="BW30" s="65"/>
+      <c r="BX30" s="65"/>
+      <c r="BY30" s="65"/>
+      <c r="BZ30" s="66"/>
     </row>
     <row r="31" spans="2:78" ht="8.25" customHeight="1">
       <c r="B31" s="3"/>
@@ -5583,72 +5580,72 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="50"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="51"/>
-      <c r="T31" s="52"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="59"/>
+      <c r="Q31" s="59"/>
+      <c r="R31" s="59"/>
+      <c r="S31" s="59"/>
+      <c r="T31" s="60"/>
       <c r="U31" s="5"/>
-      <c r="W31" s="136" t="s">
+      <c r="W31" s="138" t="s">
         <v>44</v>
       </c>
-      <c r="X31" s="137"/>
-      <c r="Y31" s="137"/>
-      <c r="Z31" s="138"/>
-      <c r="AA31" s="90" t="s">
+      <c r="X31" s="139"/>
+      <c r="Y31" s="139"/>
+      <c r="Z31" s="140"/>
+      <c r="AA31" s="98" t="s">
         <v>13</v>
       </c>
-      <c r="AB31" s="91"/>
-      <c r="AC31" s="91"/>
-      <c r="AD31" s="91"/>
-      <c r="AE31" s="91"/>
-      <c r="AF31" s="91"/>
-      <c r="AG31" s="91"/>
-      <c r="AH31" s="91"/>
-      <c r="AI31" s="92"/>
-      <c r="AJ31" s="45"/>
-      <c r="AK31" s="50"/>
-      <c r="AL31" s="51"/>
-      <c r="AM31" s="51"/>
-      <c r="AN31" s="51"/>
-      <c r="AO31" s="51"/>
-      <c r="AP31" s="52"/>
+      <c r="AB31" s="99"/>
+      <c r="AC31" s="99"/>
+      <c r="AD31" s="99"/>
+      <c r="AE31" s="99"/>
+      <c r="AF31" s="99"/>
+      <c r="AG31" s="99"/>
+      <c r="AH31" s="99"/>
+      <c r="AI31" s="100"/>
+      <c r="AJ31" s="53"/>
+      <c r="AK31" s="58"/>
+      <c r="AL31" s="59"/>
+      <c r="AM31" s="59"/>
+      <c r="AN31" s="59"/>
+      <c r="AO31" s="59"/>
+      <c r="AP31" s="60"/>
       <c r="AQ31" s="5"/>
-      <c r="AS31" s="73"/>
-      <c r="AT31" s="74"/>
-      <c r="AU31" s="74"/>
-      <c r="AV31" s="74"/>
-      <c r="AW31" s="74"/>
-      <c r="AX31" s="74"/>
-      <c r="AY31" s="74"/>
-      <c r="AZ31" s="74"/>
-      <c r="BA31" s="74"/>
-      <c r="BB31" s="74"/>
-      <c r="BC31" s="74"/>
-      <c r="BD31" s="74"/>
-      <c r="BE31" s="75"/>
-      <c r="BF31" s="45"/>
-      <c r="BG31" s="50"/>
-      <c r="BH31" s="51"/>
-      <c r="BI31" s="51"/>
-      <c r="BJ31" s="51"/>
-      <c r="BK31" s="51"/>
-      <c r="BL31" s="52"/>
+      <c r="AS31" s="81"/>
+      <c r="AT31" s="82"/>
+      <c r="AU31" s="82"/>
+      <c r="AV31" s="82"/>
+      <c r="AW31" s="82"/>
+      <c r="AX31" s="82"/>
+      <c r="AY31" s="82"/>
+      <c r="AZ31" s="82"/>
+      <c r="BA31" s="82"/>
+      <c r="BB31" s="82"/>
+      <c r="BC31" s="82"/>
+      <c r="BD31" s="82"/>
+      <c r="BE31" s="83"/>
+      <c r="BF31" s="53"/>
+      <c r="BG31" s="58"/>
+      <c r="BH31" s="59"/>
+      <c r="BI31" s="59"/>
+      <c r="BJ31" s="59"/>
+      <c r="BK31" s="59"/>
+      <c r="BL31" s="60"/>
       <c r="BM31" s="5"/>
-      <c r="BO31" s="59"/>
-      <c r="BP31" s="57"/>
-      <c r="BQ31" s="57"/>
-      <c r="BR31" s="57"/>
-      <c r="BS31" s="57"/>
-      <c r="BT31" s="57"/>
-      <c r="BU31" s="57"/>
-      <c r="BV31" s="57"/>
-      <c r="BW31" s="57"/>
-      <c r="BX31" s="57"/>
-      <c r="BY31" s="57"/>
-      <c r="BZ31" s="58"/>
+      <c r="BO31" s="67"/>
+      <c r="BP31" s="65"/>
+      <c r="BQ31" s="65"/>
+      <c r="BR31" s="65"/>
+      <c r="BS31" s="65"/>
+      <c r="BT31" s="65"/>
+      <c r="BU31" s="65"/>
+      <c r="BV31" s="65"/>
+      <c r="BW31" s="65"/>
+      <c r="BX31" s="65"/>
+      <c r="BY31" s="65"/>
+      <c r="BZ31" s="66"/>
     </row>
     <row r="32" spans="2:78" ht="15" customHeight="1">
       <c r="B32" s="3"/>
@@ -5663,70 +5660,70 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="50"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="51"/>
-      <c r="T32" s="52"/>
+      <c r="N32" s="53"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="59"/>
+      <c r="Q32" s="59"/>
+      <c r="R32" s="59"/>
+      <c r="S32" s="59"/>
+      <c r="T32" s="60"/>
       <c r="U32" s="5"/>
-      <c r="W32" s="139"/>
-      <c r="X32" s="140"/>
-      <c r="Y32" s="140"/>
-      <c r="Z32" s="141"/>
-      <c r="AA32" s="93"/>
-      <c r="AB32" s="94"/>
-      <c r="AC32" s="94"/>
-      <c r="AD32" s="94"/>
-      <c r="AE32" s="94"/>
-      <c r="AF32" s="94"/>
-      <c r="AG32" s="94"/>
-      <c r="AH32" s="94"/>
-      <c r="AI32" s="95"/>
-      <c r="AJ32" s="45"/>
-      <c r="AK32" s="50"/>
-      <c r="AL32" s="51"/>
-      <c r="AM32" s="51"/>
-      <c r="AN32" s="51"/>
-      <c r="AO32" s="51"/>
-      <c r="AP32" s="52"/>
+      <c r="W32" s="141"/>
+      <c r="X32" s="142"/>
+      <c r="Y32" s="142"/>
+      <c r="Z32" s="143"/>
+      <c r="AA32" s="101"/>
+      <c r="AB32" s="102"/>
+      <c r="AC32" s="102"/>
+      <c r="AD32" s="102"/>
+      <c r="AE32" s="102"/>
+      <c r="AF32" s="102"/>
+      <c r="AG32" s="102"/>
+      <c r="AH32" s="102"/>
+      <c r="AI32" s="103"/>
+      <c r="AJ32" s="53"/>
+      <c r="AK32" s="58"/>
+      <c r="AL32" s="59"/>
+      <c r="AM32" s="59"/>
+      <c r="AN32" s="59"/>
+      <c r="AO32" s="59"/>
+      <c r="AP32" s="60"/>
       <c r="AQ32" s="5"/>
-      <c r="AS32" s="142" t="s">
+      <c r="AS32" s="144" t="s">
         <v>19</v>
       </c>
-      <c r="AT32" s="142"/>
-      <c r="AU32" s="142"/>
-      <c r="AV32" s="142"/>
-      <c r="AW32" s="142"/>
-      <c r="AX32" s="142"/>
-      <c r="AY32" s="142"/>
-      <c r="AZ32" s="142"/>
-      <c r="BA32" s="142"/>
-      <c r="BB32" s="142"/>
-      <c r="BC32" s="142"/>
-      <c r="BD32" s="142"/>
-      <c r="BE32" s="143"/>
-      <c r="BF32" s="45"/>
-      <c r="BG32" s="50"/>
-      <c r="BH32" s="51"/>
-      <c r="BI32" s="51"/>
-      <c r="BJ32" s="51"/>
-      <c r="BK32" s="51"/>
-      <c r="BL32" s="52"/>
+      <c r="AT32" s="144"/>
+      <c r="AU32" s="144"/>
+      <c r="AV32" s="144"/>
+      <c r="AW32" s="144"/>
+      <c r="AX32" s="144"/>
+      <c r="AY32" s="144"/>
+      <c r="AZ32" s="144"/>
+      <c r="BA32" s="144"/>
+      <c r="BB32" s="144"/>
+      <c r="BC32" s="144"/>
+      <c r="BD32" s="144"/>
+      <c r="BE32" s="145"/>
+      <c r="BF32" s="53"/>
+      <c r="BG32" s="58"/>
+      <c r="BH32" s="59"/>
+      <c r="BI32" s="59"/>
+      <c r="BJ32" s="59"/>
+      <c r="BK32" s="59"/>
+      <c r="BL32" s="60"/>
       <c r="BM32" s="5"/>
-      <c r="BO32" s="59"/>
-      <c r="BP32" s="57"/>
-      <c r="BQ32" s="57"/>
-      <c r="BR32" s="57"/>
-      <c r="BS32" s="57"/>
-      <c r="BT32" s="57"/>
-      <c r="BU32" s="57"/>
-      <c r="BV32" s="57"/>
-      <c r="BW32" s="57"/>
-      <c r="BX32" s="57"/>
-      <c r="BY32" s="57"/>
-      <c r="BZ32" s="58"/>
+      <c r="BO32" s="67"/>
+      <c r="BP32" s="65"/>
+      <c r="BQ32" s="65"/>
+      <c r="BR32" s="65"/>
+      <c r="BS32" s="65"/>
+      <c r="BT32" s="65"/>
+      <c r="BU32" s="65"/>
+      <c r="BV32" s="65"/>
+      <c r="BW32" s="65"/>
+      <c r="BX32" s="65"/>
+      <c r="BY32" s="65"/>
+      <c r="BZ32" s="66"/>
     </row>
     <row r="33" spans="2:78" ht="30.75" customHeight="1">
       <c r="B33" s="3"/>
@@ -5741,72 +5738,72 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="53"/>
-      <c r="P33" s="54"/>
-      <c r="Q33" s="54"/>
-      <c r="R33" s="54"/>
-      <c r="S33" s="54"/>
-      <c r="T33" s="55"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="61"/>
+      <c r="P33" s="62"/>
+      <c r="Q33" s="62"/>
+      <c r="R33" s="62"/>
+      <c r="S33" s="62"/>
+      <c r="T33" s="63"/>
       <c r="U33" s="5"/>
-      <c r="W33" s="194" t="s">
+      <c r="W33" s="196" t="s">
         <v>40</v>
       </c>
-      <c r="X33" s="195"/>
-      <c r="Y33" s="88"/>
-      <c r="Z33" s="88"/>
-      <c r="AA33" s="88"/>
-      <c r="AB33" s="88"/>
-      <c r="AC33" s="88"/>
-      <c r="AD33" s="88"/>
-      <c r="AE33" s="88"/>
-      <c r="AF33" s="88"/>
-      <c r="AG33" s="88"/>
-      <c r="AH33" s="88"/>
-      <c r="AI33" s="89"/>
-      <c r="AJ33" s="46"/>
-      <c r="AK33" s="53"/>
-      <c r="AL33" s="54"/>
-      <c r="AM33" s="54"/>
-      <c r="AN33" s="54"/>
-      <c r="AO33" s="54"/>
-      <c r="AP33" s="55"/>
+      <c r="X33" s="197"/>
+      <c r="Y33" s="96"/>
+      <c r="Z33" s="96"/>
+      <c r="AA33" s="96"/>
+      <c r="AB33" s="96"/>
+      <c r="AC33" s="96"/>
+      <c r="AD33" s="96"/>
+      <c r="AE33" s="96"/>
+      <c r="AF33" s="96"/>
+      <c r="AG33" s="96"/>
+      <c r="AH33" s="96"/>
+      <c r="AI33" s="97"/>
+      <c r="AJ33" s="54"/>
+      <c r="AK33" s="61"/>
+      <c r="AL33" s="62"/>
+      <c r="AM33" s="62"/>
+      <c r="AN33" s="62"/>
+      <c r="AO33" s="62"/>
+      <c r="AP33" s="63"/>
       <c r="AQ33" s="5"/>
-      <c r="AS33" s="79" t="s">
+      <c r="AS33" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="AT33" s="79"/>
-      <c r="AU33" s="79"/>
-      <c r="AV33" s="79"/>
-      <c r="AW33" s="79"/>
-      <c r="AX33" s="79"/>
-      <c r="AY33" s="79"/>
-      <c r="AZ33" s="79"/>
-      <c r="BA33" s="79"/>
-      <c r="BB33" s="79"/>
-      <c r="BC33" s="79"/>
-      <c r="BD33" s="79"/>
-      <c r="BE33" s="79"/>
-      <c r="BF33" s="46"/>
-      <c r="BG33" s="53"/>
-      <c r="BH33" s="54"/>
-      <c r="BI33" s="54"/>
-      <c r="BJ33" s="54"/>
-      <c r="BK33" s="54"/>
-      <c r="BL33" s="55"/>
+      <c r="AT33" s="87"/>
+      <c r="AU33" s="87"/>
+      <c r="AV33" s="87"/>
+      <c r="AW33" s="87"/>
+      <c r="AX33" s="87"/>
+      <c r="AY33" s="87"/>
+      <c r="AZ33" s="87"/>
+      <c r="BA33" s="87"/>
+      <c r="BB33" s="87"/>
+      <c r="BC33" s="87"/>
+      <c r="BD33" s="87"/>
+      <c r="BE33" s="87"/>
+      <c r="BF33" s="54"/>
+      <c r="BG33" s="61"/>
+      <c r="BH33" s="62"/>
+      <c r="BI33" s="62"/>
+      <c r="BJ33" s="62"/>
+      <c r="BK33" s="62"/>
+      <c r="BL33" s="63"/>
       <c r="BM33" s="5"/>
-      <c r="BO33" s="60"/>
-      <c r="BP33" s="61"/>
-      <c r="BQ33" s="61"/>
-      <c r="BR33" s="61"/>
-      <c r="BS33" s="61"/>
-      <c r="BT33" s="61"/>
-      <c r="BU33" s="61"/>
-      <c r="BV33" s="61"/>
-      <c r="BW33" s="61"/>
-      <c r="BX33" s="61"/>
-      <c r="BY33" s="61"/>
-      <c r="BZ33" s="62"/>
+      <c r="BO33" s="68"/>
+      <c r="BP33" s="69"/>
+      <c r="BQ33" s="69"/>
+      <c r="BR33" s="69"/>
+      <c r="BS33" s="69"/>
+      <c r="BT33" s="69"/>
+      <c r="BU33" s="69"/>
+      <c r="BV33" s="69"/>
+      <c r="BW33" s="69"/>
+      <c r="BX33" s="69"/>
+      <c r="BY33" s="69"/>
+      <c r="BZ33" s="70"/>
     </row>
     <row r="34" spans="2:78" ht="12" customHeight="1">
       <c r="B34" s="3"/>
@@ -5821,48 +5818,48 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="43" t="s">
+      <c r="N34" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="O34" s="43"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
-      <c r="R34" s="43"/>
-      <c r="S34" s="43"/>
-      <c r="T34" s="43"/>
+      <c r="O34" s="51"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="51"/>
+      <c r="R34" s="51"/>
+      <c r="S34" s="51"/>
+      <c r="T34" s="51"/>
       <c r="U34" s="18"/>
-      <c r="AJ34" s="43" t="s">
+      <c r="AJ34" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AK34" s="43"/>
-      <c r="AL34" s="43"/>
-      <c r="AM34" s="43"/>
-      <c r="AN34" s="43"/>
-      <c r="AO34" s="43"/>
-      <c r="AP34" s="43"/>
+      <c r="AK34" s="51"/>
+      <c r="AL34" s="51"/>
+      <c r="AM34" s="51"/>
+      <c r="AN34" s="51"/>
+      <c r="AO34" s="51"/>
+      <c r="AP34" s="51"/>
       <c r="AQ34" s="18"/>
-      <c r="AS34" s="79"/>
-      <c r="AT34" s="79"/>
-      <c r="AU34" s="79"/>
-      <c r="AV34" s="79"/>
-      <c r="AW34" s="79"/>
-      <c r="AX34" s="79"/>
-      <c r="AY34" s="79"/>
-      <c r="AZ34" s="79"/>
-      <c r="BA34" s="79"/>
-      <c r="BB34" s="79"/>
-      <c r="BC34" s="79"/>
-      <c r="BD34" s="79"/>
-      <c r="BE34" s="79"/>
-      <c r="BF34" s="43" t="s">
+      <c r="AS34" s="87"/>
+      <c r="AT34" s="87"/>
+      <c r="AU34" s="87"/>
+      <c r="AV34" s="87"/>
+      <c r="AW34" s="87"/>
+      <c r="AX34" s="87"/>
+      <c r="AY34" s="87"/>
+      <c r="AZ34" s="87"/>
+      <c r="BA34" s="87"/>
+      <c r="BB34" s="87"/>
+      <c r="BC34" s="87"/>
+      <c r="BD34" s="87"/>
+      <c r="BE34" s="87"/>
+      <c r="BF34" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="BG34" s="43"/>
-      <c r="BH34" s="43"/>
-      <c r="BI34" s="43"/>
-      <c r="BJ34" s="43"/>
-      <c r="BK34" s="43"/>
-      <c r="BL34" s="43"/>
+      <c r="BG34" s="51"/>
+      <c r="BH34" s="51"/>
+      <c r="BI34" s="51"/>
+      <c r="BJ34" s="51"/>
+      <c r="BK34" s="51"/>
+      <c r="BL34" s="51"/>
       <c r="BM34" s="18"/>
     </row>
     <row r="35" spans="2:78">
@@ -5890,7 +5887,7 @@
       <c r="BM35" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="157">
+  <mergeCells count="158">
     <mergeCell ref="BP26:BW26"/>
     <mergeCell ref="W6:AD6"/>
     <mergeCell ref="AS6:AZ6"/>
@@ -5960,6 +5957,7 @@
     <mergeCell ref="AG15:AP15"/>
     <mergeCell ref="AG16:AP16"/>
     <mergeCell ref="AG17:AP17"/>
+    <mergeCell ref="BD11:BL12"/>
     <mergeCell ref="J4:T4"/>
     <mergeCell ref="J3:T3"/>
     <mergeCell ref="J2:T2"/>
@@ -5976,6 +5974,7 @@
     <mergeCell ref="W2:AD4"/>
     <mergeCell ref="W8:AG8"/>
     <mergeCell ref="B6:H6"/>
+    <mergeCell ref="BU11:BZ12"/>
     <mergeCell ref="W31:Z32"/>
     <mergeCell ref="AS32:BE32"/>
     <mergeCell ref="AS28:BE28"/>
@@ -5999,8 +5998,8 @@
     <mergeCell ref="AS13:AT18"/>
     <mergeCell ref="AS25:BJ25"/>
     <mergeCell ref="AA29:AI30"/>
-    <mergeCell ref="BD11:BL12"/>
-    <mergeCell ref="BO5:BV6"/>
+    <mergeCell ref="BF34:BL34"/>
+    <mergeCell ref="AA31:AI32"/>
     <mergeCell ref="BO7:BV9"/>
     <mergeCell ref="BW5:BZ9"/>
     <mergeCell ref="BO2:BP4"/>
@@ -6023,7 +6022,8 @@
     <mergeCell ref="BR11:BT12"/>
     <mergeCell ref="BO25:BX25"/>
     <mergeCell ref="BR10:BT10"/>
-    <mergeCell ref="BU11:BZ12"/>
+    <mergeCell ref="BO5:BR6"/>
+    <mergeCell ref="BS5:BV6"/>
     <mergeCell ref="BU10:BZ10"/>
     <mergeCell ref="K13:T14"/>
     <mergeCell ref="AG13:AP14"/>
@@ -6046,8 +6046,6 @@
     <mergeCell ref="BA19:BL19"/>
     <mergeCell ref="AS20:BL20"/>
     <mergeCell ref="AS24:BL24"/>
-    <mergeCell ref="BF34:BL34"/>
-    <mergeCell ref="AA31:AI32"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>